<commit_message>
je recommece à bosser sur ce fichier
</commit_message>
<xml_diff>
--- a/Synthese_Revision.xlsx
+++ b/Synthese_Revision.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Param_CT_RT" sheetId="1" r:id="rId1"/>
     <sheet name="NRD_Radio" sheetId="2" r:id="rId2"/>
     <sheet name="MN_Rd&amp;NRD" sheetId="4" r:id="rId3"/>
     <sheet name="MN_CQ_Gamma_cam" sheetId="5" r:id="rId4"/>
+    <sheet name="MC_CQ_TEP" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="218">
   <si>
     <t>Tension (kV)</t>
   </si>
@@ -812,6 +813,42 @@
   <si>
     <t>F 18
 FDG</t>
+  </si>
+  <si>
+    <t>But du contrôle</t>
+  </si>
+  <si>
+    <t>Trimestrielle</t>
+  </si>
+  <si>
+    <t>Param Acq</t>
+  </si>
+  <si>
+    <t>Exactitude des concentrations radioactives et calcul du SUV en mode 2D et 3D</t>
+  </si>
+  <si>
+    <t>Contrôle quotidien</t>
+  </si>
+  <si>
+    <t>Uniformité de l'image</t>
+  </si>
+  <si>
+    <t>Qualité d'image</t>
+  </si>
+  <si>
+    <t>Alignement TEP-CT</t>
+  </si>
+  <si>
+    <t>Contrôle du CT associé à l'imageur TEP</t>
+  </si>
+  <si>
+    <t>Vérification de la réponse de chaque bloc de détection
+Normalisation de la réponse des détecteurs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tolérance définie par le constructeur
+Aucun défaut sur les sinogrammes
+</t>
   </si>
 </sst>
 </file>
@@ -1253,7 +1290,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1508,6 +1545,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1529,35 +1602,23 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -1565,26 +1626,17 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1604,14 +1656,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="103">
@@ -2169,16 +2215,16 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="18" customHeight="1">
-      <c r="A4" s="103" t="s">
+      <c r="A4" s="101" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="101" t="s">
+      <c r="B4" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="90" t="s">
+      <c r="C4" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="90"/>
+      <c r="D4" s="102"/>
       <c r="E4" s="61">
         <v>0.3</v>
       </c>
@@ -2187,12 +2233,12 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" customHeight="1">
-      <c r="A5" s="103"/>
-      <c r="B5" s="101"/>
-      <c r="C5" s="99" t="s">
+      <c r="A5" s="101"/>
+      <c r="B5" s="99"/>
+      <c r="C5" s="98" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="99"/>
+      <c r="D5" s="98"/>
       <c r="E5" s="33">
         <v>1.2</v>
       </c>
@@ -2201,8 +2247,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" customHeight="1">
-      <c r="A6" s="103"/>
-      <c r="B6" s="101"/>
+      <c r="A6" s="101"/>
+      <c r="B6" s="99"/>
       <c r="C6" s="97" t="s">
         <v>22</v>
       </c>
@@ -2215,12 +2261,12 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="18" customHeight="1">
-      <c r="A7" s="103"/>
-      <c r="B7" s="101"/>
-      <c r="C7" s="98" t="s">
+      <c r="A7" s="101"/>
+      <c r="B7" s="99"/>
+      <c r="C7" s="94" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="98"/>
+      <c r="D7" s="94"/>
       <c r="E7" s="4">
         <v>9</v>
       </c>
@@ -2229,12 +2275,12 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="18" customHeight="1">
-      <c r="A8" s="103"/>
-      <c r="B8" s="101"/>
-      <c r="C8" s="90" t="s">
+      <c r="A8" s="101"/>
+      <c r="B8" s="99"/>
+      <c r="C8" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="90"/>
+      <c r="D8" s="102"/>
       <c r="E8" s="61">
         <v>4</v>
       </c>
@@ -2243,12 +2289,12 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1">
-      <c r="A9" s="103"/>
-      <c r="B9" s="101"/>
-      <c r="C9" s="98" t="s">
+      <c r="A9" s="101"/>
+      <c r="B9" s="99"/>
+      <c r="C9" s="94" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="98"/>
+      <c r="D9" s="94"/>
       <c r="E9" s="4">
         <v>4</v>
       </c>
@@ -2257,8 +2303,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="18" customHeight="1">
-      <c r="A10" s="103"/>
-      <c r="B10" s="101"/>
+      <c r="A10" s="101"/>
+      <c r="B10" s="99"/>
       <c r="C10" s="97" t="s">
         <v>26</v>
       </c>
@@ -2271,12 +2317,12 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="18" customHeight="1">
-      <c r="A11" s="103"/>
-      <c r="B11" s="101"/>
-      <c r="C11" s="99" t="s">
+      <c r="A11" s="101"/>
+      <c r="B11" s="99"/>
+      <c r="C11" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="99"/>
+      <c r="D11" s="98"/>
       <c r="E11" s="33">
         <v>7</v>
       </c>
@@ -2285,8 +2331,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="18" customHeight="1">
-      <c r="A12" s="103"/>
-      <c r="B12" s="101"/>
+      <c r="A12" s="101"/>
+      <c r="B12" s="99"/>
       <c r="C12" s="97" t="s">
         <v>28</v>
       </c>
@@ -2299,12 +2345,12 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="18" customHeight="1">
-      <c r="A13" s="103"/>
-      <c r="B13" s="101"/>
-      <c r="C13" s="99" t="s">
+      <c r="A13" s="101"/>
+      <c r="B13" s="99"/>
+      <c r="C13" s="98" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="99"/>
+      <c r="D13" s="98"/>
       <c r="E13" s="33">
         <v>25</v>
       </c>
@@ -2313,8 +2359,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="18" customHeight="1">
-      <c r="A14" s="103"/>
-      <c r="B14" s="101"/>
+      <c r="A14" s="101"/>
+      <c r="B14" s="99"/>
       <c r="C14" s="97" t="s">
         <v>30</v>
       </c>
@@ -2327,8 +2373,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="18" customHeight="1">
-      <c r="A15" s="103"/>
-      <c r="B15" s="102" t="s">
+      <c r="A15" s="101"/>
+      <c r="B15" s="100" t="s">
         <v>142</v>
       </c>
       <c r="C15" s="36" t="s">
@@ -2345,8 +2391,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="18" customHeight="1">
-      <c r="A16" s="103"/>
-      <c r="B16" s="102"/>
+      <c r="A16" s="101"/>
+      <c r="B16" s="100"/>
       <c r="C16" s="5" t="s">
         <v>143</v>
       </c>
@@ -2361,8 +2407,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="18" customHeight="1">
-      <c r="A17" s="103"/>
-      <c r="B17" s="102"/>
+      <c r="A17" s="101"/>
+      <c r="B17" s="100"/>
       <c r="C17" s="36" t="s">
         <v>144</v>
       </c>
@@ -2377,8 +2423,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="18" customHeight="1">
-      <c r="A18" s="103"/>
-      <c r="B18" s="102"/>
+      <c r="A18" s="101"/>
+      <c r="B18" s="100"/>
       <c r="C18" s="5" t="s">
         <v>144</v>
       </c>
@@ -2393,8 +2439,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="18" customHeight="1">
-      <c r="A19" s="103"/>
-      <c r="B19" s="102"/>
+      <c r="A19" s="101"/>
+      <c r="B19" s="100"/>
       <c r="C19" s="36" t="s">
         <v>145</v>
       </c>
@@ -2409,8 +2455,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="18" customHeight="1">
-      <c r="A20" s="103"/>
-      <c r="B20" s="102"/>
+      <c r="A20" s="101"/>
+      <c r="B20" s="100"/>
       <c r="C20" s="5" t="s">
         <v>145</v>
       </c>
@@ -2425,8 +2471,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="18" customHeight="1">
-      <c r="A21" s="103"/>
-      <c r="B21" s="102"/>
+      <c r="A21" s="101"/>
+      <c r="B21" s="100"/>
       <c r="C21" s="36" t="s">
         <v>146</v>
       </c>
@@ -2441,8 +2487,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="18" customHeight="1">
-      <c r="A22" s="103"/>
-      <c r="B22" s="102"/>
+      <c r="A22" s="101"/>
+      <c r="B22" s="100"/>
       <c r="C22" s="5" t="s">
         <v>146</v>
       </c>
@@ -2457,8 +2503,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="18" customHeight="1">
-      <c r="A23" s="103"/>
-      <c r="B23" s="102"/>
+      <c r="A23" s="101"/>
+      <c r="B23" s="100"/>
       <c r="C23" s="36" t="s">
         <v>146</v>
       </c>
@@ -2473,8 +2519,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="18" customHeight="1">
-      <c r="A24" s="103"/>
-      <c r="B24" s="102"/>
+      <c r="A24" s="101"/>
+      <c r="B24" s="100"/>
       <c r="C24" s="5" t="s">
         <v>22</v>
       </c>
@@ -2489,8 +2535,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="18" customHeight="1">
-      <c r="A25" s="103"/>
-      <c r="B25" s="102"/>
+      <c r="A25" s="101"/>
+      <c r="B25" s="100"/>
       <c r="C25" s="36" t="s">
         <v>22</v>
       </c>
@@ -2534,26 +2580,26 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="72" customHeight="1">
-      <c r="A30" s="104" t="s">
+      <c r="A30" s="92" t="s">
         <v>149</v>
       </c>
-      <c r="B30" s="104"/>
-      <c r="C30" s="105" t="s">
+      <c r="B30" s="92"/>
+      <c r="C30" s="93" t="s">
         <v>147</v>
       </c>
-      <c r="D30" s="105"/>
+      <c r="D30" s="93"/>
       <c r="E30" s="39">
         <v>8</v>
       </c>
       <c r="F30" s="45"/>
     </row>
     <row r="31" spans="1:6" ht="72" customHeight="1">
-      <c r="A31" s="104"/>
-      <c r="B31" s="104"/>
-      <c r="C31" s="98" t="s">
+      <c r="A31" s="92"/>
+      <c r="B31" s="92"/>
+      <c r="C31" s="94" t="s">
         <v>148</v>
       </c>
-      <c r="D31" s="98"/>
+      <c r="D31" s="94"/>
       <c r="E31" s="64"/>
       <c r="F31" s="63">
         <v>1.8</v>
@@ -2592,16 +2638,16 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="35" customHeight="1">
-      <c r="A36" s="106" t="s">
+      <c r="A36" s="96" t="s">
         <v>155</v>
       </c>
-      <c r="B36" s="96" t="s">
+      <c r="B36" s="108" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="100" t="s">
+      <c r="C36" s="95" t="s">
         <v>150</v>
       </c>
-      <c r="D36" s="100"/>
+      <c r="D36" s="95"/>
       <c r="E36" s="65">
         <v>65</v>
       </c>
@@ -2610,12 +2656,12 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="35" customHeight="1">
-      <c r="A37" s="106"/>
-      <c r="B37" s="96"/>
-      <c r="C37" s="98" t="s">
+      <c r="A37" s="96"/>
+      <c r="B37" s="108"/>
+      <c r="C37" s="94" t="s">
         <v>151</v>
       </c>
-      <c r="D37" s="98"/>
+      <c r="D37" s="94"/>
       <c r="E37" s="4">
         <v>15</v>
       </c>
@@ -2624,12 +2670,12 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="35" customHeight="1">
-      <c r="A38" s="106"/>
-      <c r="B38" s="96"/>
-      <c r="C38" s="100" t="s">
+      <c r="A38" s="96"/>
+      <c r="B38" s="108"/>
+      <c r="C38" s="95" t="s">
         <v>152</v>
       </c>
-      <c r="D38" s="100"/>
+      <c r="D38" s="95"/>
       <c r="E38" s="65">
         <v>20</v>
       </c>
@@ -2638,12 +2684,12 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="35" customHeight="1">
-      <c r="A39" s="106"/>
-      <c r="B39" s="96"/>
-      <c r="C39" s="98" t="s">
+      <c r="A39" s="96"/>
+      <c r="B39" s="108"/>
+      <c r="C39" s="94" t="s">
         <v>153</v>
       </c>
-      <c r="D39" s="98"/>
+      <c r="D39" s="94"/>
       <c r="E39" s="4">
         <v>17</v>
       </c>
@@ -2652,12 +2698,12 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="35" customHeight="1">
-      <c r="A40" s="106"/>
-      <c r="B40" s="96"/>
-      <c r="C40" s="100" t="s">
+      <c r="A40" s="96"/>
+      <c r="B40" s="108"/>
+      <c r="C40" s="95" t="s">
         <v>154</v>
       </c>
-      <c r="D40" s="100"/>
+      <c r="D40" s="95"/>
       <c r="E40" s="65">
         <v>45</v>
       </c>
@@ -2666,14 +2712,14 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="23" customHeight="1">
-      <c r="A41" s="106"/>
-      <c r="B41" s="95" t="s">
+      <c r="A41" s="96"/>
+      <c r="B41" s="107" t="s">
         <v>162</v>
       </c>
       <c r="C41" s="48" t="s">
         <v>150</v>
       </c>
-      <c r="D41" s="91">
+      <c r="D41" s="103">
         <v>10</v>
       </c>
       <c r="E41" s="57">
@@ -2684,12 +2730,12 @@
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="106"/>
-      <c r="B42" s="95"/>
+      <c r="A42" s="96"/>
+      <c r="B42" s="107"/>
       <c r="C42" t="s">
         <v>163</v>
       </c>
-      <c r="D42" s="91"/>
+      <c r="D42" s="103"/>
       <c r="E42" s="58">
         <v>25</v>
       </c>
@@ -2698,12 +2744,12 @@
       </c>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="106"/>
-      <c r="B43" s="95"/>
+      <c r="A43" s="96"/>
+      <c r="B43" s="107"/>
       <c r="C43" s="48" t="s">
         <v>164</v>
       </c>
-      <c r="D43" s="91"/>
+      <c r="D43" s="103"/>
       <c r="E43" s="57">
         <v>45</v>
       </c>
@@ -2712,12 +2758,12 @@
       </c>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="106"/>
-      <c r="B44" s="95"/>
+      <c r="A44" s="96"/>
+      <c r="B44" s="107"/>
       <c r="C44" t="s">
         <v>151</v>
       </c>
-      <c r="D44" s="91"/>
+      <c r="D44" s="103"/>
       <c r="E44" s="58">
         <v>3</v>
       </c>
@@ -2726,12 +2772,12 @@
       </c>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="106"/>
-      <c r="B45" s="95"/>
+      <c r="A45" s="96"/>
+      <c r="B45" s="107"/>
       <c r="C45" s="48" t="s">
         <v>153</v>
       </c>
-      <c r="D45" s="91"/>
+      <c r="D45" s="103"/>
       <c r="E45" s="57">
         <v>4</v>
       </c>
@@ -2740,12 +2786,12 @@
       </c>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="106"/>
-      <c r="B46" s="95"/>
+      <c r="A46" s="96"/>
+      <c r="B46" s="107"/>
       <c r="C46" s="49" t="s">
         <v>150</v>
       </c>
-      <c r="D46" s="92">
+      <c r="D46" s="104">
         <v>20</v>
       </c>
       <c r="E46" s="59">
@@ -2756,12 +2802,12 @@
       </c>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="106"/>
-      <c r="B47" s="95"/>
+      <c r="A47" s="96"/>
+      <c r="B47" s="107"/>
       <c r="C47" s="50" t="s">
         <v>163</v>
       </c>
-      <c r="D47" s="93"/>
+      <c r="D47" s="105"/>
       <c r="E47" s="57">
         <v>25</v>
       </c>
@@ -2770,12 +2816,12 @@
       </c>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="106"/>
-      <c r="B48" s="95"/>
+      <c r="A48" s="96"/>
+      <c r="B48" s="107"/>
       <c r="C48" s="51" t="s">
         <v>164</v>
       </c>
-      <c r="D48" s="93"/>
+      <c r="D48" s="105"/>
       <c r="E48" s="58">
         <v>70</v>
       </c>
@@ -2784,12 +2830,12 @@
       </c>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="106"/>
-      <c r="B49" s="95"/>
+      <c r="A49" s="96"/>
+      <c r="B49" s="107"/>
       <c r="C49" s="50" t="s">
         <v>151</v>
       </c>
-      <c r="D49" s="93"/>
+      <c r="D49" s="105"/>
       <c r="E49" s="57">
         <v>4</v>
       </c>
@@ -2798,12 +2844,12 @@
       </c>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="106"/>
-      <c r="B50" s="95"/>
+      <c r="A50" s="96"/>
+      <c r="B50" s="107"/>
       <c r="C50" s="52" t="s">
         <v>153</v>
       </c>
-      <c r="D50" s="94"/>
+      <c r="D50" s="106"/>
       <c r="E50" s="60">
         <v>5</v>
       </c>
@@ -2812,12 +2858,12 @@
       </c>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="106"/>
-      <c r="B51" s="95"/>
+      <c r="A51" s="96"/>
+      <c r="B51" s="107"/>
       <c r="C51" s="48" t="s">
         <v>150</v>
       </c>
-      <c r="D51" s="91">
+      <c r="D51" s="103">
         <v>30</v>
       </c>
       <c r="E51" s="57">
@@ -2828,12 +2874,12 @@
       </c>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="106"/>
-      <c r="B52" s="95"/>
+      <c r="A52" s="96"/>
+      <c r="B52" s="107"/>
       <c r="C52" t="s">
         <v>163</v>
       </c>
-      <c r="D52" s="91"/>
+      <c r="D52" s="103"/>
       <c r="E52" s="58">
         <v>25</v>
       </c>
@@ -2842,12 +2888,12 @@
       </c>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="106"/>
-      <c r="B53" s="95"/>
+      <c r="A53" s="96"/>
+      <c r="B53" s="107"/>
       <c r="C53" s="48" t="s">
         <v>164</v>
       </c>
-      <c r="D53" s="91"/>
+      <c r="D53" s="103"/>
       <c r="E53" s="57">
         <v>85</v>
       </c>
@@ -2856,12 +2902,12 @@
       </c>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="106"/>
-      <c r="B54" s="95"/>
+      <c r="A54" s="96"/>
+      <c r="B54" s="107"/>
       <c r="C54" t="s">
         <v>151</v>
       </c>
-      <c r="D54" s="91"/>
+      <c r="D54" s="103"/>
       <c r="E54" s="58">
         <v>5</v>
       </c>
@@ -2870,12 +2916,12 @@
       </c>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="106"/>
-      <c r="B55" s="95"/>
+      <c r="A55" s="96"/>
+      <c r="B55" s="107"/>
       <c r="C55" s="48" t="s">
         <v>153</v>
       </c>
-      <c r="D55" s="91"/>
+      <c r="D55" s="103"/>
       <c r="E55" s="57">
         <v>7</v>
       </c>
@@ -2885,6 +2931,20 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="B4:B14"/>
+    <mergeCell ref="B15:B25"/>
+    <mergeCell ref="A4:A25"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C13:D13"/>
     <mergeCell ref="A30:B31"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
@@ -2892,27 +2952,13 @@
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="A36:A55"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="B4:B14"/>
-    <mergeCell ref="B15:B25"/>
-    <mergeCell ref="A4:A25"/>
-    <mergeCell ref="C4:D4"/>
     <mergeCell ref="D41:D45"/>
     <mergeCell ref="D46:D50"/>
     <mergeCell ref="D51:D55"/>
     <mergeCell ref="B41:B55"/>
     <mergeCell ref="B36:B40"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C5:D5"/>
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C13:D13"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -2992,7 +3038,7 @@
       <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:10" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="B9" s="107" t="s">
+      <c r="B9" s="115" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="78" t="s">
@@ -3001,68 +3047,68 @@
       <c r="D9" s="78" t="s">
         <v>167</v>
       </c>
-      <c r="E9" s="112" t="s">
+      <c r="E9" s="114" t="s">
         <v>168</v>
       </c>
-      <c r="F9" s="112"/>
+      <c r="F9" s="114"/>
       <c r="G9" s="74"/>
       <c r="H9" s="74"/>
-      <c r="I9" s="115"/>
-      <c r="J9" s="115"/>
+      <c r="I9" s="109"/>
+      <c r="J9" s="109"/>
     </row>
     <row r="10" spans="1:10" s="5" customFormat="1" ht="30" customHeight="1">
-      <c r="B10" s="107"/>
+      <c r="B10" s="115"/>
       <c r="C10" s="35" t="s">
         <v>165</v>
       </c>
       <c r="D10" s="79" t="s">
         <v>171</v>
       </c>
-      <c r="E10" s="111">
+      <c r="E10" s="110">
         <v>700</v>
       </c>
-      <c r="F10" s="111"/>
+      <c r="F10" s="110"/>
     </row>
     <row r="11" spans="1:10" s="5" customFormat="1" ht="30">
-      <c r="B11" s="107"/>
+      <c r="B11" s="115"/>
       <c r="C11" s="33" t="s">
         <v>169</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E11" s="91">
+      <c r="E11" s="103">
         <v>240</v>
       </c>
-      <c r="F11" s="91"/>
+      <c r="F11" s="103"/>
     </row>
     <row r="12" spans="1:10" s="5" customFormat="1" ht="30">
-      <c r="B12" s="107"/>
-      <c r="C12" s="111" t="s">
+      <c r="B12" s="115"/>
+      <c r="C12" s="110" t="s">
         <v>170</v>
       </c>
       <c r="D12" s="79" t="s">
         <v>173</v>
       </c>
-      <c r="E12" s="111">
+      <c r="E12" s="110">
         <v>10</v>
       </c>
-      <c r="F12" s="111"/>
+      <c r="F12" s="110"/>
     </row>
     <row r="13" spans="1:10" s="5" customFormat="1" ht="30">
-      <c r="B13" s="107"/>
-      <c r="C13" s="111"/>
+      <c r="B13" s="115"/>
+      <c r="C13" s="110"/>
       <c r="D13" s="79" t="s">
         <v>174</v>
       </c>
-      <c r="E13" s="111">
+      <c r="E13" s="110">
         <v>80</v>
       </c>
-      <c r="F13" s="111"/>
+      <c r="F13" s="110"/>
     </row>
     <row r="14" spans="1:10" s="5" customFormat="1" ht="60" customHeight="1">
-      <c r="B14" s="107"/>
-      <c r="C14" s="109" t="s">
+      <c r="B14" s="115"/>
+      <c r="C14" s="111" t="s">
         <v>181</v>
       </c>
       <c r="D14" s="67" t="s">
@@ -3076,8 +3122,8 @@
       </c>
     </row>
     <row r="15" spans="1:10" s="5" customFormat="1">
-      <c r="B15" s="107"/>
-      <c r="C15" s="109"/>
+      <c r="B15" s="115"/>
+      <c r="C15" s="111"/>
       <c r="D15" s="77" t="s">
         <v>197</v>
       </c>
@@ -3089,8 +3135,8 @@
       </c>
     </row>
     <row r="16" spans="1:10" s="5" customFormat="1">
-      <c r="B16" s="107"/>
-      <c r="C16" s="109"/>
+      <c r="B16" s="115"/>
+      <c r="C16" s="111"/>
       <c r="D16" s="75" t="s">
         <v>198</v>
       </c>
@@ -3102,8 +3148,8 @@
       </c>
     </row>
     <row r="17" spans="2:9" s="5" customFormat="1" ht="30">
-      <c r="B17" s="107"/>
-      <c r="C17" s="109"/>
+      <c r="B17" s="115"/>
+      <c r="C17" s="111"/>
       <c r="D17" s="70" t="s">
         <v>175</v>
       </c>
@@ -3115,68 +3161,68 @@
       </c>
     </row>
     <row r="18" spans="2:9" s="5" customFormat="1" ht="61" customHeight="1">
-      <c r="B18" s="107"/>
+      <c r="B18" s="115"/>
       <c r="C18" s="80" t="s">
         <v>184</v>
       </c>
       <c r="D18" s="79" t="s">
         <v>176</v>
       </c>
-      <c r="E18" s="111">
+      <c r="E18" s="110">
         <v>850</v>
       </c>
-      <c r="F18" s="111"/>
+      <c r="F18" s="110"/>
     </row>
     <row r="19" spans="2:9" s="5" customFormat="1" ht="30">
-      <c r="B19" s="107"/>
-      <c r="C19" s="91" t="s">
+      <c r="B19" s="115"/>
+      <c r="C19" s="103" t="s">
         <v>185</v>
       </c>
       <c r="D19" s="73" t="s">
         <v>177</v>
       </c>
-      <c r="E19" s="94">
+      <c r="E19" s="106">
         <v>200</v>
       </c>
-      <c r="F19" s="94"/>
+      <c r="F19" s="106"/>
     </row>
     <row r="20" spans="2:9" s="5" customFormat="1" ht="30">
-      <c r="B20" s="107"/>
-      <c r="C20" s="91"/>
+      <c r="B20" s="115"/>
+      <c r="C20" s="103"/>
       <c r="D20" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="E20" s="91">
+      <c r="E20" s="103">
         <v>370</v>
       </c>
-      <c r="F20" s="91"/>
+      <c r="F20" s="103"/>
     </row>
     <row r="21" spans="2:9" s="33" customFormat="1" ht="30">
-      <c r="B21" s="107"/>
-      <c r="C21" s="114" t="s">
+      <c r="B21" s="115"/>
+      <c r="C21" s="112" t="s">
         <v>187</v>
       </c>
       <c r="D21" s="79" t="s">
         <v>186</v>
       </c>
-      <c r="E21" s="111">
+      <c r="E21" s="110">
         <v>800</v>
       </c>
-      <c r="F21" s="111"/>
+      <c r="F21" s="110"/>
     </row>
     <row r="22" spans="2:9" s="5" customFormat="1" ht="30">
-      <c r="B22" s="107"/>
-      <c r="C22" s="114"/>
+      <c r="B22" s="115"/>
+      <c r="C22" s="112"/>
       <c r="D22" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="E22" s="111">
+      <c r="E22" s="110">
         <v>500</v>
       </c>
-      <c r="F22" s="111"/>
+      <c r="F22" s="110"/>
     </row>
     <row r="23" spans="2:9" ht="30">
-      <c r="B23" s="107"/>
+      <c r="B23" s="115"/>
       <c r="C23" s="1" t="s">
         <v>188</v>
       </c>
@@ -3190,7 +3236,7 @@
     </row>
     <row r="24" spans="2:9" s="5" customFormat="1"/>
     <row r="25" spans="2:9" ht="54" customHeight="1">
-      <c r="B25" s="102" t="s">
+      <c r="B25" s="100" t="s">
         <v>142</v>
       </c>
       <c r="C25" s="83" t="s">
@@ -3216,7 +3262,7 @@
       </c>
     </row>
     <row r="26" spans="2:9" ht="30" customHeight="1">
-      <c r="B26" s="102"/>
+      <c r="B26" s="100"/>
       <c r="C26" s="81" t="s">
         <v>165</v>
       </c>
@@ -3240,7 +3286,7 @@
       </c>
     </row>
     <row r="27" spans="2:9" ht="32" customHeight="1">
-      <c r="B27" s="102"/>
+      <c r="B27" s="100"/>
       <c r="C27" s="5" t="s">
         <v>169</v>
       </c>
@@ -3264,8 +3310,8 @@
       </c>
     </row>
     <row r="28" spans="2:9" ht="32" customHeight="1">
-      <c r="B28" s="102"/>
-      <c r="C28" s="108" t="s">
+      <c r="B28" s="100"/>
+      <c r="C28" s="116" t="s">
         <v>170</v>
       </c>
       <c r="D28" s="86" t="s">
@@ -3288,8 +3334,8 @@
       </c>
     </row>
     <row r="29" spans="2:9" ht="32" customHeight="1">
-      <c r="B29" s="102"/>
-      <c r="C29" s="108"/>
+      <c r="B29" s="100"/>
+      <c r="C29" s="116"/>
       <c r="D29" s="84" t="s">
         <v>174</v>
       </c>
@@ -3310,7 +3356,7 @@
       </c>
     </row>
     <row r="30" spans="2:9" ht="47" customHeight="1">
-      <c r="B30" s="102"/>
+      <c r="B30" s="100"/>
       <c r="C30" s="67" t="s">
         <v>195</v>
       </c>
@@ -3334,7 +3380,7 @@
       </c>
     </row>
     <row r="31" spans="2:9" ht="32" customHeight="1">
-      <c r="B31" s="102"/>
+      <c r="B31" s="100"/>
       <c r="C31" s="81" t="s">
         <v>185</v>
       </c>
@@ -3358,11 +3404,11 @@
       </c>
     </row>
     <row r="32" spans="2:9" ht="30" customHeight="1">
-      <c r="B32" s="102"/>
+      <c r="B32" s="100"/>
       <c r="C32" s="85" t="s">
         <v>201</v>
       </c>
-      <c r="D32" s="109" t="s">
+      <c r="D32" s="111" t="s">
         <v>178</v>
       </c>
       <c r="E32" s="68">
@@ -3382,11 +3428,11 @@
       </c>
     </row>
     <row r="33" spans="2:9" ht="23" customHeight="1">
-      <c r="B33" s="102"/>
+      <c r="B33" s="100"/>
       <c r="C33" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="D33" s="109"/>
+      <c r="D33" s="111"/>
       <c r="E33" s="33">
         <v>20</v>
       </c>
@@ -3404,8 +3450,8 @@
       </c>
     </row>
     <row r="34" spans="2:9" ht="32" customHeight="1">
-      <c r="B34" s="102"/>
-      <c r="C34" s="110" t="s">
+      <c r="B34" s="100"/>
+      <c r="C34" s="117" t="s">
         <v>203</v>
       </c>
       <c r="D34" s="86" t="s">
@@ -3428,8 +3474,8 @@
       </c>
     </row>
     <row r="35" spans="2:9" ht="32" customHeight="1">
-      <c r="B35" s="102"/>
-      <c r="C35" s="110"/>
+      <c r="B35" s="100"/>
+      <c r="C35" s="117"/>
       <c r="D35" s="84" t="s">
         <v>204</v>
       </c>
@@ -3450,7 +3496,7 @@
       </c>
     </row>
     <row r="36" spans="2:9" ht="32" customHeight="1">
-      <c r="B36" s="102"/>
+      <c r="B36" s="100"/>
       <c r="C36" s="67" t="s">
         <v>205</v>
       </c>
@@ -3475,27 +3521,27 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B9:B23"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="B25:B36"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E20:F20"/>
     <mergeCell ref="I9:J9"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="C14:C17"/>
     <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E20:F20"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E9:F9"/>
-    <mergeCell ref="B9:B23"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="B25:B36"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -3510,8 +3556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:U16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="R6" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="O10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="U3" sqref="U3"/>
@@ -3536,48 +3582,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:21">
-      <c r="B1" s="122" t="s">
+      <c r="B1" s="118" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="122"/>
+      <c r="C1" s="118"/>
     </row>
     <row r="4" spans="2:21" s="4" customFormat="1">
-      <c r="B4" s="119" t="s">
+      <c r="B4" s="124" t="s">
         <v>118</v>
       </c>
-      <c r="C4" s="119"/>
-      <c r="D4" s="121" t="s">
+      <c r="C4" s="124"/>
+      <c r="D4" s="126" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="121"/>
-      <c r="F4" s="121"/>
-      <c r="G4" s="121"/>
-      <c r="H4" s="124" t="s">
+      <c r="E4" s="126"/>
+      <c r="F4" s="126"/>
+      <c r="G4" s="126"/>
+      <c r="H4" s="120" t="s">
         <v>119</v>
       </c>
-      <c r="I4" s="124"/>
-      <c r="J4" s="124"/>
-      <c r="K4" s="124"/>
-      <c r="L4" s="124"/>
-      <c r="M4" s="120" t="s">
+      <c r="I4" s="120"/>
+      <c r="J4" s="120"/>
+      <c r="K4" s="120"/>
+      <c r="L4" s="120"/>
+      <c r="M4" s="125" t="s">
         <v>120</v>
       </c>
-      <c r="N4" s="120"/>
-      <c r="O4" s="120"/>
-      <c r="P4" s="120"/>
-      <c r="Q4" s="120"/>
-      <c r="R4" s="120"/>
-      <c r="S4" s="116" t="s">
+      <c r="N4" s="125"/>
+      <c r="O4" s="125"/>
+      <c r="P4" s="125"/>
+      <c r="Q4" s="125"/>
+      <c r="R4" s="125"/>
+      <c r="S4" s="121" t="s">
         <v>121</v>
       </c>
-      <c r="T4" s="116"/>
-      <c r="U4" s="116"/>
+      <c r="T4" s="121"/>
+      <c r="U4" s="121"/>
     </row>
     <row r="5" spans="2:21" s="7" customFormat="1" ht="60">
-      <c r="B5" s="123" t="s">
+      <c r="B5" s="119" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="123"/>
+      <c r="C5" s="119"/>
       <c r="D5" s="8" t="s">
         <v>39</v>
       </c>
@@ -3634,10 +3680,10 @@
       </c>
     </row>
     <row r="6" spans="2:21" s="11" customFormat="1">
-      <c r="B6" s="123" t="s">
+      <c r="B6" s="119" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="123"/>
+      <c r="C6" s="119"/>
       <c r="D6" s="12" t="s">
         <v>45</v>
       </c>
@@ -3694,10 +3740,10 @@
       </c>
     </row>
     <row r="7" spans="2:21" s="11" customFormat="1" ht="75">
-      <c r="B7" s="123" t="s">
+      <c r="B7" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="123"/>
+      <c r="C7" s="119"/>
       <c r="D7" s="13" t="s">
         <v>50</v>
       </c>
@@ -3754,10 +3800,10 @@
       </c>
     </row>
     <row r="8" spans="2:21" s="15" customFormat="1" ht="60">
-      <c r="B8" s="123" t="s">
+      <c r="B8" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="123"/>
+      <c r="C8" s="119"/>
       <c r="D8" s="14" t="s">
         <v>48</v>
       </c>
@@ -3808,10 +3854,10 @@
       </c>
     </row>
     <row r="9" spans="2:21" s="15" customFormat="1" ht="142" customHeight="1">
-      <c r="B9" s="123" t="s">
+      <c r="B9" s="119" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="123"/>
+      <c r="C9" s="119"/>
       <c r="D9" s="14" t="s">
         <v>61</v>
       </c>
@@ -3868,10 +3914,10 @@
       </c>
     </row>
     <row r="10" spans="2:21" s="18" customFormat="1">
-      <c r="B10" s="119" t="s">
+      <c r="B10" s="124" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="119"/>
+      <c r="C10" s="124"/>
       <c r="D10" s="16">
         <v>512</v>
       </c>
@@ -3920,10 +3966,10 @@
       </c>
     </row>
     <row r="11" spans="2:21" s="18" customFormat="1">
-      <c r="B11" s="117" t="s">
+      <c r="B11" s="122" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="118"/>
+      <c r="C11" s="123"/>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
       <c r="F11" s="23"/>
@@ -3968,10 +4014,10 @@
       </c>
     </row>
     <row r="12" spans="2:21" s="18" customFormat="1">
-      <c r="B12" s="117" t="s">
+      <c r="B12" s="122" t="s">
         <v>82</v>
       </c>
-      <c r="C12" s="118"/>
+      <c r="C12" s="123"/>
       <c r="D12" s="24" t="s">
         <v>84</v>
       </c>
@@ -4026,10 +4072,10 @@
       </c>
     </row>
     <row r="13" spans="2:21" s="18" customFormat="1">
-      <c r="B13" s="119" t="s">
+      <c r="B13" s="124" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="119"/>
+      <c r="C13" s="124"/>
       <c r="D13" s="16" t="s">
         <v>58</v>
       </c>
@@ -4080,7 +4126,7 @@
       </c>
     </row>
     <row r="14" spans="2:21" s="18" customFormat="1" ht="30">
-      <c r="B14" s="119" t="s">
+      <c r="B14" s="124" t="s">
         <v>35</v>
       </c>
       <c r="C14" s="31" t="s">
@@ -4120,7 +4166,7 @@
       <c r="U14" s="17"/>
     </row>
     <row r="15" spans="2:21" s="10" customFormat="1" ht="105">
-      <c r="B15" s="119"/>
+      <c r="B15" s="124"/>
       <c r="C15" s="32" t="s">
         <v>132</v>
       </c>
@@ -4162,10 +4208,10 @@
       </c>
     </row>
     <row r="16" spans="2:21" s="10" customFormat="1" ht="45">
-      <c r="B16" s="119" t="s">
+      <c r="B16" s="124" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="119"/>
+      <c r="C16" s="124"/>
       <c r="D16" s="19" t="s">
         <v>55</v>
       </c>
@@ -4217,13 +4263,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="H4:L4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
     <mergeCell ref="S4:U4"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B14:B15"/>
@@ -4234,6 +4273,13 @@
     <mergeCell ref="M4:R4"/>
     <mergeCell ref="D4:G4"/>
     <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="H4:L4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -4242,4 +4288,103 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:H9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="90"/>
+    <col min="2" max="2" width="19" style="90" customWidth="1"/>
+    <col min="3" max="3" width="39.33203125" style="90" customWidth="1"/>
+    <col min="4" max="4" width="34.1640625" style="90" customWidth="1"/>
+    <col min="5" max="9" width="16.33203125" style="90" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="90"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:8">
+      <c r="B3" s="90" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="90" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="90" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="45">
+      <c r="B4" s="90" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="91" t="s">
+        <v>211</v>
+      </c>
+      <c r="D4" s="91" t="s">
+        <v>210</v>
+      </c>
+      <c r="E4" s="90" t="s">
+        <v>212</v>
+      </c>
+      <c r="F4" s="90" t="s">
+        <v>213</v>
+      </c>
+      <c r="G4" s="90" t="s">
+        <v>214</v>
+      </c>
+      <c r="H4" s="90" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="45">
+      <c r="B5" s="90" t="s">
+        <v>207</v>
+      </c>
+      <c r="C5" s="127" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="B6" s="90" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="90" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="45">
+      <c r="B7" s="90" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="127" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="B8" s="90" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="90" t="s">
+        <v>209</v>
+      </c>
+      <c r="B9" s="90" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
travail en cours ajout d'une partie TEP
</commit_message>
<xml_diff>
--- a/Synthese_Revision.xlsx
+++ b/Synthese_Revision.xlsx
@@ -11,7 +11,7 @@
     <sheet name="NRD_Radio" sheetId="2" r:id="rId2"/>
     <sheet name="MN_Rd&amp;NRD" sheetId="4" r:id="rId3"/>
     <sheet name="MN_CQ_Gamma_cam" sheetId="5" r:id="rId4"/>
-    <sheet name="MC_CQ_TEP" sheetId="6" r:id="rId5"/>
+    <sheet name="MN_CQ_TEP" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="229">
   <si>
     <t>Tension (kV)</t>
   </si>
@@ -839,9 +839,6 @@
     <t>Alignement TEP-CT</t>
   </si>
   <si>
-    <t>Contrôle du CT associé à l'imageur TEP</t>
-  </si>
-  <si>
     <t>Vérification de la réponse de chaque bloc de détection
 Normalisation de la réponse des détecteurs</t>
   </si>
@@ -849,6 +846,57 @@
     <t xml:space="preserve">Tolérance définie par le constructeur
 Aucun défaut sur les sinogrammes
 </t>
+  </si>
+  <si>
+    <t>Réglementation
+Recomandation</t>
+  </si>
+  <si>
+    <t>Vérification de l'uniformité radiale en mode 3D dans le champ de vue du tomographe</t>
+  </si>
+  <si>
+    <t>Evaluation de la précision des corrections apporter aux données acquises</t>
+  </si>
+  <si>
+    <t>Evaluation de la qualité d'image dans les conditions cliniques</t>
+  </si>
+  <si>
+    <t>Contrôle du recalage des origines des axes des 2 statifs TEP et TDM
+Vérifier la superposisition des images acquises</t>
+  </si>
+  <si>
+    <t>Contrôle du CT associé à l'imageur TEP (Mensuelle selon la SFPM)</t>
+  </si>
+  <si>
+    <t>Ge 68</t>
+  </si>
+  <si>
+    <t>Positionnement de la source de Ge 68 dans l'imageur
+Paramètre suivi: nb coïncidence, nb single, dead time, timing, spectrometrie
+Utilisation du protocole constructeur pour réaliser et analyser acquisition
++ Analyse visuelle de la qualité d'image</t>
+  </si>
+  <si>
+    <t>F 18 ou Ge 68</t>
+  </si>
+  <si>
+    <t>Fantôme de PMMA cylindrique de 20 cm de diamètre + fluor 18
+(possibilité avec fantôme de Ge 68)
+Positionnement du fantôme en bout de table
+réalisation d'un topogramme -&gt; CT du fanôme
+Acquisition TEP
+reconstruction 
+analyse des images reconstruites avec corrections d'attenuation</t>
+  </si>
+  <si>
+    <t>SUV doit être égale à 1± 5%
+Avec un coefficient de variation inférieure à 10% pour les valeurs relevées sur les différentes coupes</t>
+  </si>
+  <si>
+    <t>Fantôme de PMMA cylindrique de 20 cm de diamètre + fluor 18
+(possibilité avec fantôme de Ge 68)
+Acquisition TEP d'1h
+Réalisation d'anneaux concentriques de surface identique  sur plusieurs coupes</t>
   </si>
 </sst>
 </file>
@@ -926,7 +974,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1014,6 +1062,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1185,7 +1251,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="103">
+  <cellStyleXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1289,8 +1355,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1551,39 +1619,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1602,32 +1670,50 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1638,29 +1724,38 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="103">
+  <cellStyles count="105">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -1712,6 +1807,7 @@
     <cellStyle name="Lien hypertexte" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="103" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -1763,6 +1859,7 @@
     <cellStyle name="Lien hypertexte visité" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="104" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2215,16 +2312,16 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="18" customHeight="1">
-      <c r="A4" s="101" t="s">
+      <c r="A4" s="96" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="99" t="s">
+      <c r="B4" s="94" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="102" t="s">
+      <c r="C4" s="97" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="102"/>
+      <c r="D4" s="97"/>
       <c r="E4" s="61">
         <v>0.3</v>
       </c>
@@ -2233,12 +2330,12 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" customHeight="1">
-      <c r="A5" s="101"/>
-      <c r="B5" s="99"/>
-      <c r="C5" s="98" t="s">
+      <c r="A5" s="96"/>
+      <c r="B5" s="94"/>
+      <c r="C5" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="98"/>
+      <c r="D5" s="93"/>
       <c r="E5" s="33">
         <v>1.2</v>
       </c>
@@ -2247,12 +2344,12 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" customHeight="1">
-      <c r="A6" s="101"/>
-      <c r="B6" s="99"/>
-      <c r="C6" s="97" t="s">
+      <c r="A6" s="96"/>
+      <c r="B6" s="94"/>
+      <c r="C6" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="97"/>
+      <c r="D6" s="92"/>
       <c r="E6" s="35">
         <v>8</v>
       </c>
@@ -2261,12 +2358,12 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="18" customHeight="1">
-      <c r="A7" s="101"/>
-      <c r="B7" s="99"/>
-      <c r="C7" s="94" t="s">
+      <c r="A7" s="96"/>
+      <c r="B7" s="94"/>
+      <c r="C7" s="98" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="94"/>
+      <c r="D7" s="98"/>
       <c r="E7" s="4">
         <v>9</v>
       </c>
@@ -2275,12 +2372,12 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="18" customHeight="1">
-      <c r="A8" s="101"/>
-      <c r="B8" s="99"/>
-      <c r="C8" s="102" t="s">
+      <c r="A8" s="96"/>
+      <c r="B8" s="94"/>
+      <c r="C8" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="102"/>
+      <c r="D8" s="97"/>
       <c r="E8" s="61">
         <v>4</v>
       </c>
@@ -2289,12 +2386,12 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1">
-      <c r="A9" s="101"/>
-      <c r="B9" s="99"/>
-      <c r="C9" s="94" t="s">
+      <c r="A9" s="96"/>
+      <c r="B9" s="94"/>
+      <c r="C9" s="98" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="94"/>
+      <c r="D9" s="98"/>
       <c r="E9" s="4">
         <v>4</v>
       </c>
@@ -2303,12 +2400,12 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="18" customHeight="1">
-      <c r="A10" s="101"/>
-      <c r="B10" s="99"/>
-      <c r="C10" s="97" t="s">
+      <c r="A10" s="96"/>
+      <c r="B10" s="94"/>
+      <c r="C10" s="92" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="97"/>
+      <c r="D10" s="92"/>
       <c r="E10" s="35">
         <v>5</v>
       </c>
@@ -2317,12 +2414,12 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="18" customHeight="1">
-      <c r="A11" s="101"/>
-      <c r="B11" s="99"/>
-      <c r="C11" s="98" t="s">
+      <c r="A11" s="96"/>
+      <c r="B11" s="94"/>
+      <c r="C11" s="93" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="98"/>
+      <c r="D11" s="93"/>
       <c r="E11" s="33">
         <v>7</v>
       </c>
@@ -2331,12 +2428,12 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="18" customHeight="1">
-      <c r="A12" s="101"/>
-      <c r="B12" s="99"/>
-      <c r="C12" s="97" t="s">
+      <c r="A12" s="96"/>
+      <c r="B12" s="94"/>
+      <c r="C12" s="92" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="97"/>
+      <c r="D12" s="92"/>
       <c r="E12" s="35">
         <v>10</v>
       </c>
@@ -2345,12 +2442,12 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="18" customHeight="1">
-      <c r="A13" s="101"/>
-      <c r="B13" s="99"/>
-      <c r="C13" s="98" t="s">
+      <c r="A13" s="96"/>
+      <c r="B13" s="94"/>
+      <c r="C13" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="98"/>
+      <c r="D13" s="93"/>
       <c r="E13" s="33">
         <v>25</v>
       </c>
@@ -2359,12 +2456,12 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="18" customHeight="1">
-      <c r="A14" s="101"/>
-      <c r="B14" s="99"/>
-      <c r="C14" s="97" t="s">
+      <c r="A14" s="96"/>
+      <c r="B14" s="94"/>
+      <c r="C14" s="92" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="97"/>
+      <c r="D14" s="92"/>
       <c r="E14" s="35" t="s">
         <v>31</v>
       </c>
@@ -2373,8 +2470,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="18" customHeight="1">
-      <c r="A15" s="101"/>
-      <c r="B15" s="100" t="s">
+      <c r="A15" s="96"/>
+      <c r="B15" s="95" t="s">
         <v>142</v>
       </c>
       <c r="C15" s="36" t="s">
@@ -2391,8 +2488,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="18" customHeight="1">
-      <c r="A16" s="101"/>
-      <c r="B16" s="100"/>
+      <c r="A16" s="96"/>
+      <c r="B16" s="95"/>
       <c r="C16" s="5" t="s">
         <v>143</v>
       </c>
@@ -2407,8 +2504,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="18" customHeight="1">
-      <c r="A17" s="101"/>
-      <c r="B17" s="100"/>
+      <c r="A17" s="96"/>
+      <c r="B17" s="95"/>
       <c r="C17" s="36" t="s">
         <v>144</v>
       </c>
@@ -2423,8 +2520,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="18" customHeight="1">
-      <c r="A18" s="101"/>
-      <c r="B18" s="100"/>
+      <c r="A18" s="96"/>
+      <c r="B18" s="95"/>
       <c r="C18" s="5" t="s">
         <v>144</v>
       </c>
@@ -2439,8 +2536,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="18" customHeight="1">
-      <c r="A19" s="101"/>
-      <c r="B19" s="100"/>
+      <c r="A19" s="96"/>
+      <c r="B19" s="95"/>
       <c r="C19" s="36" t="s">
         <v>145</v>
       </c>
@@ -2455,8 +2552,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="18" customHeight="1">
-      <c r="A20" s="101"/>
-      <c r="B20" s="100"/>
+      <c r="A20" s="96"/>
+      <c r="B20" s="95"/>
       <c r="C20" s="5" t="s">
         <v>145</v>
       </c>
@@ -2471,8 +2568,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="18" customHeight="1">
-      <c r="A21" s="101"/>
-      <c r="B21" s="100"/>
+      <c r="A21" s="96"/>
+      <c r="B21" s="95"/>
       <c r="C21" s="36" t="s">
         <v>146</v>
       </c>
@@ -2487,8 +2584,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="18" customHeight="1">
-      <c r="A22" s="101"/>
-      <c r="B22" s="100"/>
+      <c r="A22" s="96"/>
+      <c r="B22" s="95"/>
       <c r="C22" s="5" t="s">
         <v>146</v>
       </c>
@@ -2503,8 +2600,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="18" customHeight="1">
-      <c r="A23" s="101"/>
-      <c r="B23" s="100"/>
+      <c r="A23" s="96"/>
+      <c r="B23" s="95"/>
       <c r="C23" s="36" t="s">
         <v>146</v>
       </c>
@@ -2519,8 +2616,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="18" customHeight="1">
-      <c r="A24" s="101"/>
-      <c r="B24" s="100"/>
+      <c r="A24" s="96"/>
+      <c r="B24" s="95"/>
       <c r="C24" s="5" t="s">
         <v>22</v>
       </c>
@@ -2535,8 +2632,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="18" customHeight="1">
-      <c r="A25" s="101"/>
-      <c r="B25" s="100"/>
+      <c r="A25" s="96"/>
+      <c r="B25" s="95"/>
       <c r="C25" s="36" t="s">
         <v>22</v>
       </c>
@@ -2580,26 +2677,26 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="72" customHeight="1">
-      <c r="A30" s="92" t="s">
+      <c r="A30" s="99" t="s">
         <v>149</v>
       </c>
-      <c r="B30" s="92"/>
-      <c r="C30" s="93" t="s">
+      <c r="B30" s="99"/>
+      <c r="C30" s="100" t="s">
         <v>147</v>
       </c>
-      <c r="D30" s="93"/>
+      <c r="D30" s="100"/>
       <c r="E30" s="39">
         <v>8</v>
       </c>
       <c r="F30" s="45"/>
     </row>
     <row r="31" spans="1:6" ht="72" customHeight="1">
-      <c r="A31" s="92"/>
-      <c r="B31" s="92"/>
-      <c r="C31" s="94" t="s">
+      <c r="A31" s="99"/>
+      <c r="B31" s="99"/>
+      <c r="C31" s="98" t="s">
         <v>148</v>
       </c>
-      <c r="D31" s="94"/>
+      <c r="D31" s="98"/>
       <c r="E31" s="64"/>
       <c r="F31" s="63">
         <v>1.8</v>
@@ -2638,16 +2735,16 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="35" customHeight="1">
-      <c r="A36" s="96" t="s">
+      <c r="A36" s="102" t="s">
         <v>155</v>
       </c>
       <c r="B36" s="108" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="95" t="s">
+      <c r="C36" s="101" t="s">
         <v>150</v>
       </c>
-      <c r="D36" s="95"/>
+      <c r="D36" s="101"/>
       <c r="E36" s="65">
         <v>65</v>
       </c>
@@ -2656,12 +2753,12 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="35" customHeight="1">
-      <c r="A37" s="96"/>
+      <c r="A37" s="102"/>
       <c r="B37" s="108"/>
-      <c r="C37" s="94" t="s">
+      <c r="C37" s="98" t="s">
         <v>151</v>
       </c>
-      <c r="D37" s="94"/>
+      <c r="D37" s="98"/>
       <c r="E37" s="4">
         <v>15</v>
       </c>
@@ -2670,12 +2767,12 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="35" customHeight="1">
-      <c r="A38" s="96"/>
+      <c r="A38" s="102"/>
       <c r="B38" s="108"/>
-      <c r="C38" s="95" t="s">
+      <c r="C38" s="101" t="s">
         <v>152</v>
       </c>
-      <c r="D38" s="95"/>
+      <c r="D38" s="101"/>
       <c r="E38" s="65">
         <v>20</v>
       </c>
@@ -2684,12 +2781,12 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="35" customHeight="1">
-      <c r="A39" s="96"/>
+      <c r="A39" s="102"/>
       <c r="B39" s="108"/>
-      <c r="C39" s="94" t="s">
+      <c r="C39" s="98" t="s">
         <v>153</v>
       </c>
-      <c r="D39" s="94"/>
+      <c r="D39" s="98"/>
       <c r="E39" s="4">
         <v>17</v>
       </c>
@@ -2698,12 +2795,12 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="35" customHeight="1">
-      <c r="A40" s="96"/>
+      <c r="A40" s="102"/>
       <c r="B40" s="108"/>
-      <c r="C40" s="95" t="s">
+      <c r="C40" s="101" t="s">
         <v>154</v>
       </c>
-      <c r="D40" s="95"/>
+      <c r="D40" s="101"/>
       <c r="E40" s="65">
         <v>45</v>
       </c>
@@ -2712,7 +2809,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="23" customHeight="1">
-      <c r="A41" s="96"/>
+      <c r="A41" s="102"/>
       <c r="B41" s="107" t="s">
         <v>162</v>
       </c>
@@ -2730,7 +2827,7 @@
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="96"/>
+      <c r="A42" s="102"/>
       <c r="B42" s="107"/>
       <c r="C42" t="s">
         <v>163</v>
@@ -2744,7 +2841,7 @@
       </c>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="96"/>
+      <c r="A43" s="102"/>
       <c r="B43" s="107"/>
       <c r="C43" s="48" t="s">
         <v>164</v>
@@ -2758,7 +2855,7 @@
       </c>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="96"/>
+      <c r="A44" s="102"/>
       <c r="B44" s="107"/>
       <c r="C44" t="s">
         <v>151</v>
@@ -2772,7 +2869,7 @@
       </c>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="96"/>
+      <c r="A45" s="102"/>
       <c r="B45" s="107"/>
       <c r="C45" s="48" t="s">
         <v>153</v>
@@ -2786,7 +2883,7 @@
       </c>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="96"/>
+      <c r="A46" s="102"/>
       <c r="B46" s="107"/>
       <c r="C46" s="49" t="s">
         <v>150</v>
@@ -2802,7 +2899,7 @@
       </c>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="96"/>
+      <c r="A47" s="102"/>
       <c r="B47" s="107"/>
       <c r="C47" s="50" t="s">
         <v>163</v>
@@ -2816,7 +2913,7 @@
       </c>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="96"/>
+      <c r="A48" s="102"/>
       <c r="B48" s="107"/>
       <c r="C48" s="51" t="s">
         <v>164</v>
@@ -2830,7 +2927,7 @@
       </c>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="96"/>
+      <c r="A49" s="102"/>
       <c r="B49" s="107"/>
       <c r="C49" s="50" t="s">
         <v>151</v>
@@ -2844,7 +2941,7 @@
       </c>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="96"/>
+      <c r="A50" s="102"/>
       <c r="B50" s="107"/>
       <c r="C50" s="52" t="s">
         <v>153</v>
@@ -2858,7 +2955,7 @@
       </c>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="96"/>
+      <c r="A51" s="102"/>
       <c r="B51" s="107"/>
       <c r="C51" s="48" t="s">
         <v>150</v>
@@ -2874,7 +2971,7 @@
       </c>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="96"/>
+      <c r="A52" s="102"/>
       <c r="B52" s="107"/>
       <c r="C52" t="s">
         <v>163</v>
@@ -2888,7 +2985,7 @@
       </c>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="96"/>
+      <c r="A53" s="102"/>
       <c r="B53" s="107"/>
       <c r="C53" s="48" t="s">
         <v>164</v>
@@ -2902,7 +2999,7 @@
       </c>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="96"/>
+      <c r="A54" s="102"/>
       <c r="B54" s="107"/>
       <c r="C54" t="s">
         <v>151</v>
@@ -2916,7 +3013,7 @@
       </c>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="96"/>
+      <c r="A55" s="102"/>
       <c r="B55" s="107"/>
       <c r="C55" s="48" t="s">
         <v>153</v>
@@ -2931,6 +3028,20 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A30:B31"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A36:A55"/>
+    <mergeCell ref="D41:D45"/>
+    <mergeCell ref="D46:D50"/>
+    <mergeCell ref="D51:D55"/>
+    <mergeCell ref="B41:B55"/>
+    <mergeCell ref="B36:B40"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C36:D36"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="B4:B14"/>
@@ -2945,20 +3056,6 @@
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A30:B31"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A36:A55"/>
-    <mergeCell ref="D41:D45"/>
-    <mergeCell ref="D46:D50"/>
-    <mergeCell ref="D51:D55"/>
-    <mergeCell ref="B41:B55"/>
-    <mergeCell ref="B36:B40"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C36:D36"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -3038,7 +3135,7 @@
       <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:10" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="B9" s="115" t="s">
+      <c r="B9" s="109" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="78" t="s">
@@ -3047,30 +3144,30 @@
       <c r="D9" s="78" t="s">
         <v>167</v>
       </c>
-      <c r="E9" s="114" t="s">
+      <c r="E9" s="117" t="s">
         <v>168</v>
       </c>
-      <c r="F9" s="114"/>
+      <c r="F9" s="117"/>
       <c r="G9" s="74"/>
       <c r="H9" s="74"/>
-      <c r="I9" s="109"/>
-      <c r="J9" s="109"/>
+      <c r="I9" s="116"/>
+      <c r="J9" s="116"/>
     </row>
     <row r="10" spans="1:10" s="5" customFormat="1" ht="30" customHeight="1">
-      <c r="B10" s="115"/>
+      <c r="B10" s="109"/>
       <c r="C10" s="35" t="s">
         <v>165</v>
       </c>
       <c r="D10" s="79" t="s">
         <v>171</v>
       </c>
-      <c r="E10" s="110">
+      <c r="E10" s="115">
         <v>700</v>
       </c>
-      <c r="F10" s="110"/>
+      <c r="F10" s="115"/>
     </row>
     <row r="11" spans="1:10" s="5" customFormat="1" ht="30">
-      <c r="B11" s="115"/>
+      <c r="B11" s="109"/>
       <c r="C11" s="33" t="s">
         <v>169</v>
       </c>
@@ -3083,31 +3180,31 @@
       <c r="F11" s="103"/>
     </row>
     <row r="12" spans="1:10" s="5" customFormat="1" ht="30">
-      <c r="B12" s="115"/>
-      <c r="C12" s="110" t="s">
+      <c r="B12" s="109"/>
+      <c r="C12" s="115" t="s">
         <v>170</v>
       </c>
       <c r="D12" s="79" t="s">
         <v>173</v>
       </c>
-      <c r="E12" s="110">
+      <c r="E12" s="115">
         <v>10</v>
       </c>
-      <c r="F12" s="110"/>
+      <c r="F12" s="115"/>
     </row>
     <row r="13" spans="1:10" s="5" customFormat="1" ht="30">
-      <c r="B13" s="115"/>
-      <c r="C13" s="110"/>
+      <c r="B13" s="109"/>
+      <c r="C13" s="115"/>
       <c r="D13" s="79" t="s">
         <v>174</v>
       </c>
-      <c r="E13" s="110">
+      <c r="E13" s="115">
         <v>80</v>
       </c>
-      <c r="F13" s="110"/>
+      <c r="F13" s="115"/>
     </row>
     <row r="14" spans="1:10" s="5" customFormat="1" ht="60" customHeight="1">
-      <c r="B14" s="115"/>
+      <c r="B14" s="109"/>
       <c r="C14" s="111" t="s">
         <v>181</v>
       </c>
@@ -3122,7 +3219,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" s="5" customFormat="1">
-      <c r="B15" s="115"/>
+      <c r="B15" s="109"/>
       <c r="C15" s="111"/>
       <c r="D15" s="77" t="s">
         <v>197</v>
@@ -3135,7 +3232,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" s="5" customFormat="1">
-      <c r="B16" s="115"/>
+      <c r="B16" s="109"/>
       <c r="C16" s="111"/>
       <c r="D16" s="75" t="s">
         <v>198</v>
@@ -3148,7 +3245,7 @@
       </c>
     </row>
     <row r="17" spans="2:9" s="5" customFormat="1" ht="30">
-      <c r="B17" s="115"/>
+      <c r="B17" s="109"/>
       <c r="C17" s="111"/>
       <c r="D17" s="70" t="s">
         <v>175</v>
@@ -3161,20 +3258,20 @@
       </c>
     </row>
     <row r="18" spans="2:9" s="5" customFormat="1" ht="61" customHeight="1">
-      <c r="B18" s="115"/>
+      <c r="B18" s="109"/>
       <c r="C18" s="80" t="s">
         <v>184</v>
       </c>
       <c r="D18" s="79" t="s">
         <v>176</v>
       </c>
-      <c r="E18" s="110">
+      <c r="E18" s="115">
         <v>850</v>
       </c>
-      <c r="F18" s="110"/>
+      <c r="F18" s="115"/>
     </row>
     <row r="19" spans="2:9" s="5" customFormat="1" ht="30">
-      <c r="B19" s="115"/>
+      <c r="B19" s="109"/>
       <c r="C19" s="103" t="s">
         <v>185</v>
       </c>
@@ -3187,7 +3284,7 @@
       <c r="F19" s="106"/>
     </row>
     <row r="20" spans="2:9" s="5" customFormat="1" ht="30">
-      <c r="B20" s="115"/>
+      <c r="B20" s="109"/>
       <c r="C20" s="103"/>
       <c r="D20" s="2" t="s">
         <v>178</v>
@@ -3198,45 +3295,45 @@
       <c r="F20" s="103"/>
     </row>
     <row r="21" spans="2:9" s="33" customFormat="1" ht="30">
-      <c r="B21" s="115"/>
-      <c r="C21" s="112" t="s">
+      <c r="B21" s="109"/>
+      <c r="C21" s="113" t="s">
         <v>187</v>
       </c>
       <c r="D21" s="79" t="s">
         <v>186</v>
       </c>
-      <c r="E21" s="110">
+      <c r="E21" s="115">
         <v>800</v>
       </c>
-      <c r="F21" s="110"/>
+      <c r="F21" s="115"/>
     </row>
     <row r="22" spans="2:9" s="5" customFormat="1" ht="30">
-      <c r="B22" s="115"/>
-      <c r="C22" s="112"/>
+      <c r="B22" s="109"/>
+      <c r="C22" s="113"/>
       <c r="D22" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="E22" s="110">
+      <c r="E22" s="115">
         <v>500</v>
       </c>
-      <c r="F22" s="110"/>
+      <c r="F22" s="115"/>
     </row>
     <row r="23" spans="2:9" ht="30">
-      <c r="B23" s="115"/>
+      <c r="B23" s="109"/>
       <c r="C23" s="1" t="s">
         <v>188</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E23" s="113">
+      <c r="E23" s="114">
         <v>350</v>
       </c>
-      <c r="F23" s="113"/>
+      <c r="F23" s="114"/>
     </row>
     <row r="24" spans="2:9" s="5" customFormat="1"/>
     <row r="25" spans="2:9" ht="54" customHeight="1">
-      <c r="B25" s="100" t="s">
+      <c r="B25" s="95" t="s">
         <v>142</v>
       </c>
       <c r="C25" s="83" t="s">
@@ -3262,7 +3359,7 @@
       </c>
     </row>
     <row r="26" spans="2:9" ht="30" customHeight="1">
-      <c r="B26" s="100"/>
+      <c r="B26" s="95"/>
       <c r="C26" s="81" t="s">
         <v>165</v>
       </c>
@@ -3286,7 +3383,7 @@
       </c>
     </row>
     <row r="27" spans="2:9" ht="32" customHeight="1">
-      <c r="B27" s="100"/>
+      <c r="B27" s="95"/>
       <c r="C27" s="5" t="s">
         <v>169</v>
       </c>
@@ -3310,8 +3407,8 @@
       </c>
     </row>
     <row r="28" spans="2:9" ht="32" customHeight="1">
-      <c r="B28" s="100"/>
-      <c r="C28" s="116" t="s">
+      <c r="B28" s="95"/>
+      <c r="C28" s="110" t="s">
         <v>170</v>
       </c>
       <c r="D28" s="86" t="s">
@@ -3334,8 +3431,8 @@
       </c>
     </row>
     <row r="29" spans="2:9" ht="32" customHeight="1">
-      <c r="B29" s="100"/>
-      <c r="C29" s="116"/>
+      <c r="B29" s="95"/>
+      <c r="C29" s="110"/>
       <c r="D29" s="84" t="s">
         <v>174</v>
       </c>
@@ -3356,7 +3453,7 @@
       </c>
     </row>
     <row r="30" spans="2:9" ht="47" customHeight="1">
-      <c r="B30" s="100"/>
+      <c r="B30" s="95"/>
       <c r="C30" s="67" t="s">
         <v>195</v>
       </c>
@@ -3380,7 +3477,7 @@
       </c>
     </row>
     <row r="31" spans="2:9" ht="32" customHeight="1">
-      <c r="B31" s="100"/>
+      <c r="B31" s="95"/>
       <c r="C31" s="81" t="s">
         <v>185</v>
       </c>
@@ -3404,7 +3501,7 @@
       </c>
     </row>
     <row r="32" spans="2:9" ht="30" customHeight="1">
-      <c r="B32" s="100"/>
+      <c r="B32" s="95"/>
       <c r="C32" s="85" t="s">
         <v>201</v>
       </c>
@@ -3428,7 +3525,7 @@
       </c>
     </row>
     <row r="33" spans="2:9" ht="23" customHeight="1">
-      <c r="B33" s="100"/>
+      <c r="B33" s="95"/>
       <c r="C33" s="5" t="s">
         <v>202</v>
       </c>
@@ -3450,8 +3547,8 @@
       </c>
     </row>
     <row r="34" spans="2:9" ht="32" customHeight="1">
-      <c r="B34" s="100"/>
-      <c r="C34" s="117" t="s">
+      <c r="B34" s="95"/>
+      <c r="C34" s="112" t="s">
         <v>203</v>
       </c>
       <c r="D34" s="86" t="s">
@@ -3474,8 +3571,8 @@
       </c>
     </row>
     <row r="35" spans="2:9" ht="32" customHeight="1">
-      <c r="B35" s="100"/>
-      <c r="C35" s="117"/>
+      <c r="B35" s="95"/>
+      <c r="C35" s="112"/>
       <c r="D35" s="84" t="s">
         <v>204</v>
       </c>
@@ -3496,7 +3593,7 @@
       </c>
     </row>
     <row r="36" spans="2:9" ht="32" customHeight="1">
-      <c r="B36" s="100"/>
+      <c r="B36" s="95"/>
       <c r="C36" s="67" t="s">
         <v>205</v>
       </c>
@@ -3521,27 +3618,27 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E9:F9"/>
     <mergeCell ref="B9:B23"/>
     <mergeCell ref="C28:C29"/>
     <mergeCell ref="D32:D33"/>
     <mergeCell ref="C34:C35"/>
     <mergeCell ref="B25:B36"/>
     <mergeCell ref="C21:C22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="E18:F18"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="C14:C17"/>
     <mergeCell ref="C19:C20"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E9:F9"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -3560,7 +3657,7 @@
       <pane xSplit="3" ySplit="5" topLeftCell="O10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="U3" sqref="U3"/>
+      <selection pane="bottomRight" activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3582,48 +3679,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:21">
-      <c r="B1" s="118" t="s">
+      <c r="B1" s="124" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="118"/>
+      <c r="C1" s="124"/>
     </row>
     <row r="4" spans="2:21" s="4" customFormat="1">
-      <c r="B4" s="124" t="s">
+      <c r="B4" s="121" t="s">
         <v>118</v>
       </c>
-      <c r="C4" s="124"/>
-      <c r="D4" s="126" t="s">
+      <c r="C4" s="121"/>
+      <c r="D4" s="123" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="126"/>
-      <c r="F4" s="126"/>
-      <c r="G4" s="126"/>
-      <c r="H4" s="120" t="s">
+      <c r="E4" s="123"/>
+      <c r="F4" s="123"/>
+      <c r="G4" s="123"/>
+      <c r="H4" s="126" t="s">
         <v>119</v>
       </c>
-      <c r="I4" s="120"/>
-      <c r="J4" s="120"/>
-      <c r="K4" s="120"/>
-      <c r="L4" s="120"/>
-      <c r="M4" s="125" t="s">
+      <c r="I4" s="126"/>
+      <c r="J4" s="126"/>
+      <c r="K4" s="126"/>
+      <c r="L4" s="126"/>
+      <c r="M4" s="122" t="s">
         <v>120</v>
       </c>
-      <c r="N4" s="125"/>
-      <c r="O4" s="125"/>
-      <c r="P4" s="125"/>
-      <c r="Q4" s="125"/>
-      <c r="R4" s="125"/>
-      <c r="S4" s="121" t="s">
+      <c r="N4" s="122"/>
+      <c r="O4" s="122"/>
+      <c r="P4" s="122"/>
+      <c r="Q4" s="122"/>
+      <c r="R4" s="122"/>
+      <c r="S4" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="T4" s="121"/>
-      <c r="U4" s="121"/>
+      <c r="T4" s="118"/>
+      <c r="U4" s="118"/>
     </row>
     <row r="5" spans="2:21" s="7" customFormat="1" ht="60">
-      <c r="B5" s="119" t="s">
+      <c r="B5" s="125" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="119"/>
+      <c r="C5" s="125"/>
       <c r="D5" s="8" t="s">
         <v>39</v>
       </c>
@@ -3680,10 +3777,10 @@
       </c>
     </row>
     <row r="6" spans="2:21" s="11" customFormat="1">
-      <c r="B6" s="119" t="s">
+      <c r="B6" s="125" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="119"/>
+      <c r="C6" s="125"/>
       <c r="D6" s="12" t="s">
         <v>45</v>
       </c>
@@ -3740,10 +3837,10 @@
       </c>
     </row>
     <row r="7" spans="2:21" s="11" customFormat="1" ht="75">
-      <c r="B7" s="119" t="s">
+      <c r="B7" s="125" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="119"/>
+      <c r="C7" s="125"/>
       <c r="D7" s="13" t="s">
         <v>50</v>
       </c>
@@ -3800,10 +3897,10 @@
       </c>
     </row>
     <row r="8" spans="2:21" s="15" customFormat="1" ht="60">
-      <c r="B8" s="119" t="s">
+      <c r="B8" s="125" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="119"/>
+      <c r="C8" s="125"/>
       <c r="D8" s="14" t="s">
         <v>48</v>
       </c>
@@ -3854,10 +3951,10 @@
       </c>
     </row>
     <row r="9" spans="2:21" s="15" customFormat="1" ht="142" customHeight="1">
-      <c r="B9" s="119" t="s">
+      <c r="B9" s="125" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="119"/>
+      <c r="C9" s="125"/>
       <c r="D9" s="14" t="s">
         <v>61</v>
       </c>
@@ -3914,10 +4011,10 @@
       </c>
     </row>
     <row r="10" spans="2:21" s="18" customFormat="1">
-      <c r="B10" s="124" t="s">
+      <c r="B10" s="121" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="124"/>
+      <c r="C10" s="121"/>
       <c r="D10" s="16">
         <v>512</v>
       </c>
@@ -3966,10 +4063,10 @@
       </c>
     </row>
     <row r="11" spans="2:21" s="18" customFormat="1">
-      <c r="B11" s="122" t="s">
+      <c r="B11" s="119" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="123"/>
+      <c r="C11" s="120"/>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
       <c r="F11" s="23"/>
@@ -4014,10 +4111,10 @@
       </c>
     </row>
     <row r="12" spans="2:21" s="18" customFormat="1">
-      <c r="B12" s="122" t="s">
+      <c r="B12" s="119" t="s">
         <v>82</v>
       </c>
-      <c r="C12" s="123"/>
+      <c r="C12" s="120"/>
       <c r="D12" s="24" t="s">
         <v>84</v>
       </c>
@@ -4072,10 +4169,10 @@
       </c>
     </row>
     <row r="13" spans="2:21" s="18" customFormat="1">
-      <c r="B13" s="124" t="s">
+      <c r="B13" s="121" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="124"/>
+      <c r="C13" s="121"/>
       <c r="D13" s="16" t="s">
         <v>58</v>
       </c>
@@ -4126,7 +4223,7 @@
       </c>
     </row>
     <row r="14" spans="2:21" s="18" customFormat="1" ht="30">
-      <c r="B14" s="124" t="s">
+      <c r="B14" s="121" t="s">
         <v>35</v>
       </c>
       <c r="C14" s="31" t="s">
@@ -4166,7 +4263,7 @@
       <c r="U14" s="17"/>
     </row>
     <row r="15" spans="2:21" s="10" customFormat="1" ht="105">
-      <c r="B15" s="124"/>
+      <c r="B15" s="121"/>
       <c r="C15" s="32" t="s">
         <v>132</v>
       </c>
@@ -4208,10 +4305,10 @@
       </c>
     </row>
     <row r="16" spans="2:21" s="10" customFormat="1" ht="45">
-      <c r="B16" s="124" t="s">
+      <c r="B16" s="121" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="124"/>
+      <c r="C16" s="121"/>
       <c r="D16" s="19" t="s">
         <v>55</v>
       </c>
@@ -4263,6 +4360,13 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="H4:L4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
     <mergeCell ref="S4:U4"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B14:B15"/>
@@ -4273,13 +4377,6 @@
     <mergeCell ref="M4:R4"/>
     <mergeCell ref="D4:G4"/>
     <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="H4:L4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -4294,93 +4391,162 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="90"/>
-    <col min="2" max="2" width="19" style="90" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" style="90" customWidth="1"/>
     <col min="3" max="3" width="39.33203125" style="90" customWidth="1"/>
-    <col min="4" max="4" width="34.1640625" style="90" customWidth="1"/>
-    <col min="5" max="9" width="16.33203125" style="90" customWidth="1"/>
+    <col min="4" max="4" width="39.5" style="90" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" style="90" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" style="90" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" style="90" customWidth="1"/>
+    <col min="8" max="8" width="21.5" style="90" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" style="90" customWidth="1"/>
     <col min="10" max="16384" width="10.83203125" style="90"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:8">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="127" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="90" t="s">
+      <c r="C3" s="128" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="90" t="s">
+      <c r="D3" s="129" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="45">
-      <c r="B4" s="90" t="s">
+      <c r="E3" s="129"/>
+      <c r="F3" s="129"/>
+      <c r="G3" s="129"/>
+      <c r="H3" s="129"/>
+    </row>
+    <row r="4" spans="1:8" s="91" customFormat="1" ht="60">
+      <c r="B4" s="130" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="91" t="s">
+      <c r="C4" s="25" t="s">
         <v>211</v>
       </c>
-      <c r="D4" s="91" t="s">
+      <c r="D4" s="131" t="s">
         <v>210</v>
       </c>
-      <c r="E4" s="90" t="s">
+      <c r="E4" s="131" t="s">
         <v>212</v>
       </c>
-      <c r="F4" s="90" t="s">
+      <c r="F4" s="131" t="s">
         <v>213</v>
       </c>
-      <c r="G4" s="90" t="s">
+      <c r="G4" s="131" t="s">
         <v>214</v>
       </c>
-      <c r="H4" s="90" t="s">
+      <c r="H4" s="131" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="75">
+      <c r="B5" s="127" t="s">
+        <v>207</v>
+      </c>
+      <c r="C5" s="132" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="45">
-      <c r="B5" s="90" t="s">
-        <v>207</v>
-      </c>
-      <c r="C5" s="127" t="s">
+      <c r="D5" s="133" t="s">
+        <v>219</v>
+      </c>
+      <c r="E5" s="133" t="s">
+        <v>218</v>
+      </c>
+      <c r="F5" s="133" t="s">
+        <v>220</v>
+      </c>
+      <c r="G5" s="134" t="s">
+        <v>221</v>
+      </c>
+      <c r="H5" s="135"/>
+    </row>
+    <row r="6" spans="1:8" ht="30">
+      <c r="B6" s="130" t="s">
+        <v>217</v>
+      </c>
+      <c r="C6" s="135" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="135" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="135" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="135" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="135" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="135" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="60">
+      <c r="B7" s="127" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="136" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="B6" s="90" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="90" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="45">
-      <c r="B7" s="90" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="127" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="B8" s="90" t="s">
+      <c r="D7" s="136" t="s">
+        <v>227</v>
+      </c>
+      <c r="E7" s="135"/>
+      <c r="F7" s="135"/>
+      <c r="G7" s="135"/>
+      <c r="H7" s="135"/>
+    </row>
+    <row r="8" spans="1:8" ht="150">
+      <c r="B8" s="127" t="s">
         <v>60</v>
       </c>
+      <c r="C8" s="136" t="s">
+        <v>224</v>
+      </c>
+      <c r="D8" s="136" t="s">
+        <v>226</v>
+      </c>
+      <c r="E8" s="136" t="s">
+        <v>228</v>
+      </c>
+      <c r="F8" s="135"/>
+      <c r="G8" s="135"/>
+      <c r="H8" s="135"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="90" t="s">
         <v>209</v>
       </c>
-      <c r="B9" s="90" t="s">
+      <c r="B9" s="127" t="s">
         <v>82</v>
       </c>
+      <c r="C9" s="135" t="s">
+        <v>223</v>
+      </c>
+      <c r="D9" s="135" t="s">
+        <v>225</v>
+      </c>
+      <c r="E9" s="135"/>
+      <c r="F9" s="135"/>
+      <c r="G9" s="135"/>
+      <c r="H9" s="135"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D3:H3"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
ajout MN CQ TEP
</commit_message>
<xml_diff>
--- a/Synthese_Revision.xlsx
+++ b/Synthese_Revision.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="236">
   <si>
     <t>Tension (kV)</t>
   </si>
@@ -249,6 +249,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
       <t>-&lt;ROI&gt;)))</t>
@@ -591,6 +592,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
       <t>pour épaisseur de sein de 45 mm (40 mm de PMMA) en numérique</t>
@@ -628,6 +630,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
@@ -863,9 +866,6 @@
   <si>
     <t>Contrôle du recalage des origines des axes des 2 statifs TEP et TDM
 Vérifier la superposisition des images acquises</t>
-  </si>
-  <si>
-    <t>Contrôle du CT associé à l'imageur TEP (Mensuelle selon la SFPM)</t>
   </si>
   <si>
     <t>Ge 68</t>
@@ -897,6 +897,38 @@
 (possibilité avec fantôme de Ge 68)
 Acquisition TEP d'1h
 Réalisation d'anneaux concentriques de surface identique  sur plusieurs coupes</t>
+  </si>
+  <si>
+    <t>Fantôme type IEC avec sphères de différents diamètres pour un rapport 4 et un rapport 8
+Mesure des coefficients de recouvremement</t>
+  </si>
+  <si>
+    <t>Contrôle du CT associé à l'imageur TEP (Mensuel selon la SFPM)</t>
+  </si>
+  <si>
+    <t>F 18</t>
+  </si>
+  <si>
+    <t>Tolérance fixée par le constructeur</t>
+  </si>
+  <si>
+    <t>Utilisation 2 lignes source positionné dans un rectangle en diagonal de manière à ce qu'elle se croise (Siemens)
+Comme les lignes sont radio opaques et sources possibilités d'images les lignes sources en TEP et en CT pour ensuite determinés leurs coordonnées dans les 2 référentielles. On mesurera les ecart grâce à la fusion des images
+Utilisation de 5 billes radio opaques acquisition possible en CT et en TEP avec source de Ge 68 intergré (Vieille TEPGE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acquisition d'images du fantôme équivalent eau du constructeur
+Alignement du fantôme en bout de table: Acquisition pour 70 kV, 110 kV et 130 kV
+1 Roi centrale et 4 Roi périphérique
+Relevé de la moyenne et de l'ecart type des pixels de ces ROI
+</t>
+  </si>
+  <si>
+    <t>Nombre CT moyen ROI centrale ± 4 UH
+Nombre CT moyen ROI périphérique : nbCT Roi centrale ± 4 UH</t>
+  </si>
+  <si>
+    <t>Vérification du nombre Hounsfield de l'eau sur le CT</t>
   </si>
 </sst>
 </file>
@@ -909,6 +941,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1358,7 +1391,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1619,6 +1652,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1637,38 +1730,17 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -1685,36 +1757,6 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1724,35 +1766,41 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="105">
@@ -2312,16 +2360,16 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="18" customHeight="1">
-      <c r="A4" s="96" t="s">
+      <c r="A4" s="116" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="94" t="s">
+      <c r="B4" s="114" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="97" t="s">
+      <c r="C4" s="117" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="97"/>
+      <c r="D4" s="117"/>
       <c r="E4" s="61">
         <v>0.3</v>
       </c>
@@ -2330,12 +2378,12 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" customHeight="1">
-      <c r="A5" s="96"/>
-      <c r="B5" s="94"/>
-      <c r="C5" s="93" t="s">
+      <c r="A5" s="116"/>
+      <c r="B5" s="114"/>
+      <c r="C5" s="113" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="93"/>
+      <c r="D5" s="113"/>
       <c r="E5" s="33">
         <v>1.2</v>
       </c>
@@ -2344,12 +2392,12 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" customHeight="1">
-      <c r="A6" s="96"/>
-      <c r="B6" s="94"/>
-      <c r="C6" s="92" t="s">
+      <c r="A6" s="116"/>
+      <c r="B6" s="114"/>
+      <c r="C6" s="112" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="92"/>
+      <c r="D6" s="112"/>
       <c r="E6" s="35">
         <v>8</v>
       </c>
@@ -2358,12 +2406,12 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="18" customHeight="1">
-      <c r="A7" s="96"/>
-      <c r="B7" s="94"/>
-      <c r="C7" s="98" t="s">
+      <c r="A7" s="116"/>
+      <c r="B7" s="114"/>
+      <c r="C7" s="103" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="98"/>
+      <c r="D7" s="103"/>
       <c r="E7" s="4">
         <v>9</v>
       </c>
@@ -2372,12 +2420,12 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="18" customHeight="1">
-      <c r="A8" s="96"/>
-      <c r="B8" s="94"/>
-      <c r="C8" s="97" t="s">
+      <c r="A8" s="116"/>
+      <c r="B8" s="114"/>
+      <c r="C8" s="117" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="97"/>
+      <c r="D8" s="117"/>
       <c r="E8" s="61">
         <v>4</v>
       </c>
@@ -2386,12 +2434,12 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1">
-      <c r="A9" s="96"/>
-      <c r="B9" s="94"/>
-      <c r="C9" s="98" t="s">
+      <c r="A9" s="116"/>
+      <c r="B9" s="114"/>
+      <c r="C9" s="103" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="98"/>
+      <c r="D9" s="103"/>
       <c r="E9" s="4">
         <v>4</v>
       </c>
@@ -2400,12 +2448,12 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="18" customHeight="1">
-      <c r="A10" s="96"/>
-      <c r="B10" s="94"/>
-      <c r="C10" s="92" t="s">
+      <c r="A10" s="116"/>
+      <c r="B10" s="114"/>
+      <c r="C10" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="92"/>
+      <c r="D10" s="112"/>
       <c r="E10" s="35">
         <v>5</v>
       </c>
@@ -2414,12 +2462,12 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="18" customHeight="1">
-      <c r="A11" s="96"/>
-      <c r="B11" s="94"/>
-      <c r="C11" s="93" t="s">
+      <c r="A11" s="116"/>
+      <c r="B11" s="114"/>
+      <c r="C11" s="113" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="93"/>
+      <c r="D11" s="113"/>
       <c r="E11" s="33">
         <v>7</v>
       </c>
@@ -2428,12 +2476,12 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="18" customHeight="1">
-      <c r="A12" s="96"/>
-      <c r="B12" s="94"/>
-      <c r="C12" s="92" t="s">
+      <c r="A12" s="116"/>
+      <c r="B12" s="114"/>
+      <c r="C12" s="112" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="92"/>
+      <c r="D12" s="112"/>
       <c r="E12" s="35">
         <v>10</v>
       </c>
@@ -2442,12 +2490,12 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="18" customHeight="1">
-      <c r="A13" s="96"/>
-      <c r="B13" s="94"/>
-      <c r="C13" s="93" t="s">
+      <c r="A13" s="116"/>
+      <c r="B13" s="114"/>
+      <c r="C13" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="93"/>
+      <c r="D13" s="113"/>
       <c r="E13" s="33">
         <v>25</v>
       </c>
@@ -2456,12 +2504,12 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="18" customHeight="1">
-      <c r="A14" s="96"/>
-      <c r="B14" s="94"/>
-      <c r="C14" s="92" t="s">
+      <c r="A14" s="116"/>
+      <c r="B14" s="114"/>
+      <c r="C14" s="112" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="92"/>
+      <c r="D14" s="112"/>
       <c r="E14" s="35" t="s">
         <v>31</v>
       </c>
@@ -2470,8 +2518,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="18" customHeight="1">
-      <c r="A15" s="96"/>
-      <c r="B15" s="95" t="s">
+      <c r="A15" s="116"/>
+      <c r="B15" s="115" t="s">
         <v>142</v>
       </c>
       <c r="C15" s="36" t="s">
@@ -2488,8 +2536,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="18" customHeight="1">
-      <c r="A16" s="96"/>
-      <c r="B16" s="95"/>
+      <c r="A16" s="116"/>
+      <c r="B16" s="115"/>
       <c r="C16" s="5" t="s">
         <v>143</v>
       </c>
@@ -2504,8 +2552,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="18" customHeight="1">
-      <c r="A17" s="96"/>
-      <c r="B17" s="95"/>
+      <c r="A17" s="116"/>
+      <c r="B17" s="115"/>
       <c r="C17" s="36" t="s">
         <v>144</v>
       </c>
@@ -2520,8 +2568,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="18" customHeight="1">
-      <c r="A18" s="96"/>
-      <c r="B18" s="95"/>
+      <c r="A18" s="116"/>
+      <c r="B18" s="115"/>
       <c r="C18" s="5" t="s">
         <v>144</v>
       </c>
@@ -2536,8 +2584,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="18" customHeight="1">
-      <c r="A19" s="96"/>
-      <c r="B19" s="95"/>
+      <c r="A19" s="116"/>
+      <c r="B19" s="115"/>
       <c r="C19" s="36" t="s">
         <v>145</v>
       </c>
@@ -2552,8 +2600,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="18" customHeight="1">
-      <c r="A20" s="96"/>
-      <c r="B20" s="95"/>
+      <c r="A20" s="116"/>
+      <c r="B20" s="115"/>
       <c r="C20" s="5" t="s">
         <v>145</v>
       </c>
@@ -2568,8 +2616,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="18" customHeight="1">
-      <c r="A21" s="96"/>
-      <c r="B21" s="95"/>
+      <c r="A21" s="116"/>
+      <c r="B21" s="115"/>
       <c r="C21" s="36" t="s">
         <v>146</v>
       </c>
@@ -2584,8 +2632,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="18" customHeight="1">
-      <c r="A22" s="96"/>
-      <c r="B22" s="95"/>
+      <c r="A22" s="116"/>
+      <c r="B22" s="115"/>
       <c r="C22" s="5" t="s">
         <v>146</v>
       </c>
@@ -2600,8 +2648,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="18" customHeight="1">
-      <c r="A23" s="96"/>
-      <c r="B23" s="95"/>
+      <c r="A23" s="116"/>
+      <c r="B23" s="115"/>
       <c r="C23" s="36" t="s">
         <v>146</v>
       </c>
@@ -2616,8 +2664,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="18" customHeight="1">
-      <c r="A24" s="96"/>
-      <c r="B24" s="95"/>
+      <c r="A24" s="116"/>
+      <c r="B24" s="115"/>
       <c r="C24" s="5" t="s">
         <v>22</v>
       </c>
@@ -2632,8 +2680,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="18" customHeight="1">
-      <c r="A25" s="96"/>
-      <c r="B25" s="95"/>
+      <c r="A25" s="116"/>
+      <c r="B25" s="115"/>
       <c r="C25" s="36" t="s">
         <v>22</v>
       </c>
@@ -2677,26 +2725,26 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="72" customHeight="1">
-      <c r="A30" s="99" t="s">
+      <c r="A30" s="101" t="s">
         <v>149</v>
       </c>
-      <c r="B30" s="99"/>
-      <c r="C30" s="100" t="s">
+      <c r="B30" s="101"/>
+      <c r="C30" s="102" t="s">
         <v>147</v>
       </c>
-      <c r="D30" s="100"/>
+      <c r="D30" s="102"/>
       <c r="E30" s="39">
         <v>8</v>
       </c>
       <c r="F30" s="45"/>
     </row>
     <row r="31" spans="1:6" ht="72" customHeight="1">
-      <c r="A31" s="99"/>
-      <c r="B31" s="99"/>
-      <c r="C31" s="98" t="s">
+      <c r="A31" s="101"/>
+      <c r="B31" s="101"/>
+      <c r="C31" s="103" t="s">
         <v>148</v>
       </c>
-      <c r="D31" s="98"/>
+      <c r="D31" s="103"/>
       <c r="E31" s="64"/>
       <c r="F31" s="63">
         <v>1.8</v>
@@ -2735,16 +2783,16 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="35" customHeight="1">
-      <c r="A36" s="102" t="s">
+      <c r="A36" s="105" t="s">
         <v>155</v>
       </c>
-      <c r="B36" s="108" t="s">
+      <c r="B36" s="111" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="101" t="s">
+      <c r="C36" s="104" t="s">
         <v>150</v>
       </c>
-      <c r="D36" s="101"/>
+      <c r="D36" s="104"/>
       <c r="E36" s="65">
         <v>65</v>
       </c>
@@ -2753,12 +2801,12 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="35" customHeight="1">
-      <c r="A37" s="102"/>
-      <c r="B37" s="108"/>
-      <c r="C37" s="98" t="s">
+      <c r="A37" s="105"/>
+      <c r="B37" s="111"/>
+      <c r="C37" s="103" t="s">
         <v>151</v>
       </c>
-      <c r="D37" s="98"/>
+      <c r="D37" s="103"/>
       <c r="E37" s="4">
         <v>15</v>
       </c>
@@ -2767,12 +2815,12 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="35" customHeight="1">
-      <c r="A38" s="102"/>
-      <c r="B38" s="108"/>
-      <c r="C38" s="101" t="s">
+      <c r="A38" s="105"/>
+      <c r="B38" s="111"/>
+      <c r="C38" s="104" t="s">
         <v>152</v>
       </c>
-      <c r="D38" s="101"/>
+      <c r="D38" s="104"/>
       <c r="E38" s="65">
         <v>20</v>
       </c>
@@ -2781,12 +2829,12 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="35" customHeight="1">
-      <c r="A39" s="102"/>
-      <c r="B39" s="108"/>
-      <c r="C39" s="98" t="s">
+      <c r="A39" s="105"/>
+      <c r="B39" s="111"/>
+      <c r="C39" s="103" t="s">
         <v>153</v>
       </c>
-      <c r="D39" s="98"/>
+      <c r="D39" s="103"/>
       <c r="E39" s="4">
         <v>17</v>
       </c>
@@ -2795,12 +2843,12 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="35" customHeight="1">
-      <c r="A40" s="102"/>
-      <c r="B40" s="108"/>
-      <c r="C40" s="101" t="s">
+      <c r="A40" s="105"/>
+      <c r="B40" s="111"/>
+      <c r="C40" s="104" t="s">
         <v>154</v>
       </c>
-      <c r="D40" s="101"/>
+      <c r="D40" s="104"/>
       <c r="E40" s="65">
         <v>45</v>
       </c>
@@ -2809,14 +2857,14 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="23" customHeight="1">
-      <c r="A41" s="102"/>
-      <c r="B41" s="107" t="s">
+      <c r="A41" s="105"/>
+      <c r="B41" s="110" t="s">
         <v>162</v>
       </c>
       <c r="C41" s="48" t="s">
         <v>150</v>
       </c>
-      <c r="D41" s="103">
+      <c r="D41" s="106">
         <v>10</v>
       </c>
       <c r="E41" s="57">
@@ -2827,12 +2875,12 @@
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="102"/>
-      <c r="B42" s="107"/>
+      <c r="A42" s="105"/>
+      <c r="B42" s="110"/>
       <c r="C42" t="s">
         <v>163</v>
       </c>
-      <c r="D42" s="103"/>
+      <c r="D42" s="106"/>
       <c r="E42" s="58">
         <v>25</v>
       </c>
@@ -2841,12 +2889,12 @@
       </c>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="102"/>
-      <c r="B43" s="107"/>
+      <c r="A43" s="105"/>
+      <c r="B43" s="110"/>
       <c r="C43" s="48" t="s">
         <v>164</v>
       </c>
-      <c r="D43" s="103"/>
+      <c r="D43" s="106"/>
       <c r="E43" s="57">
         <v>45</v>
       </c>
@@ -2855,12 +2903,12 @@
       </c>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="102"/>
-      <c r="B44" s="107"/>
+      <c r="A44" s="105"/>
+      <c r="B44" s="110"/>
       <c r="C44" t="s">
         <v>151</v>
       </c>
-      <c r="D44" s="103"/>
+      <c r="D44" s="106"/>
       <c r="E44" s="58">
         <v>3</v>
       </c>
@@ -2869,12 +2917,12 @@
       </c>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="102"/>
-      <c r="B45" s="107"/>
+      <c r="A45" s="105"/>
+      <c r="B45" s="110"/>
       <c r="C45" s="48" t="s">
         <v>153</v>
       </c>
-      <c r="D45" s="103"/>
+      <c r="D45" s="106"/>
       <c r="E45" s="57">
         <v>4</v>
       </c>
@@ -2883,12 +2931,12 @@
       </c>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="102"/>
-      <c r="B46" s="107"/>
+      <c r="A46" s="105"/>
+      <c r="B46" s="110"/>
       <c r="C46" s="49" t="s">
         <v>150</v>
       </c>
-      <c r="D46" s="104">
+      <c r="D46" s="107">
         <v>20</v>
       </c>
       <c r="E46" s="59">
@@ -2899,12 +2947,12 @@
       </c>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="102"/>
-      <c r="B47" s="107"/>
+      <c r="A47" s="105"/>
+      <c r="B47" s="110"/>
       <c r="C47" s="50" t="s">
         <v>163</v>
       </c>
-      <c r="D47" s="105"/>
+      <c r="D47" s="108"/>
       <c r="E47" s="57">
         <v>25</v>
       </c>
@@ -2913,12 +2961,12 @@
       </c>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="102"/>
-      <c r="B48" s="107"/>
+      <c r="A48" s="105"/>
+      <c r="B48" s="110"/>
       <c r="C48" s="51" t="s">
         <v>164</v>
       </c>
-      <c r="D48" s="105"/>
+      <c r="D48" s="108"/>
       <c r="E48" s="58">
         <v>70</v>
       </c>
@@ -2927,12 +2975,12 @@
       </c>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="102"/>
-      <c r="B49" s="107"/>
+      <c r="A49" s="105"/>
+      <c r="B49" s="110"/>
       <c r="C49" s="50" t="s">
         <v>151</v>
       </c>
-      <c r="D49" s="105"/>
+      <c r="D49" s="108"/>
       <c r="E49" s="57">
         <v>4</v>
       </c>
@@ -2941,12 +2989,12 @@
       </c>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="102"/>
-      <c r="B50" s="107"/>
+      <c r="A50" s="105"/>
+      <c r="B50" s="110"/>
       <c r="C50" s="52" t="s">
         <v>153</v>
       </c>
-      <c r="D50" s="106"/>
+      <c r="D50" s="109"/>
       <c r="E50" s="60">
         <v>5</v>
       </c>
@@ -2955,12 +3003,12 @@
       </c>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="102"/>
-      <c r="B51" s="107"/>
+      <c r="A51" s="105"/>
+      <c r="B51" s="110"/>
       <c r="C51" s="48" t="s">
         <v>150</v>
       </c>
-      <c r="D51" s="103">
+      <c r="D51" s="106">
         <v>30</v>
       </c>
       <c r="E51" s="57">
@@ -2971,12 +3019,12 @@
       </c>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="102"/>
-      <c r="B52" s="107"/>
+      <c r="A52" s="105"/>
+      <c r="B52" s="110"/>
       <c r="C52" t="s">
         <v>163</v>
       </c>
-      <c r="D52" s="103"/>
+      <c r="D52" s="106"/>
       <c r="E52" s="58">
         <v>25</v>
       </c>
@@ -2985,12 +3033,12 @@
       </c>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="102"/>
-      <c r="B53" s="107"/>
+      <c r="A53" s="105"/>
+      <c r="B53" s="110"/>
       <c r="C53" s="48" t="s">
         <v>164</v>
       </c>
-      <c r="D53" s="103"/>
+      <c r="D53" s="106"/>
       <c r="E53" s="57">
         <v>85</v>
       </c>
@@ -2999,12 +3047,12 @@
       </c>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="102"/>
-      <c r="B54" s="107"/>
+      <c r="A54" s="105"/>
+      <c r="B54" s="110"/>
       <c r="C54" t="s">
         <v>151</v>
       </c>
-      <c r="D54" s="103"/>
+      <c r="D54" s="106"/>
       <c r="E54" s="58">
         <v>5</v>
       </c>
@@ -3013,12 +3061,12 @@
       </c>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="102"/>
-      <c r="B55" s="107"/>
+      <c r="A55" s="105"/>
+      <c r="B55" s="110"/>
       <c r="C55" s="48" t="s">
         <v>153</v>
       </c>
-      <c r="D55" s="103"/>
+      <c r="D55" s="106"/>
       <c r="E55" s="57">
         <v>7</v>
       </c>
@@ -3028,6 +3076,20 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="B4:B14"/>
+    <mergeCell ref="B15:B25"/>
+    <mergeCell ref="A4:A25"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C13:D13"/>
     <mergeCell ref="A30:B31"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
@@ -3042,20 +3104,6 @@
     <mergeCell ref="B36:B40"/>
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="B4:B14"/>
-    <mergeCell ref="B15:B25"/>
-    <mergeCell ref="A4:A25"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C13:D13"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -3135,7 +3183,7 @@
       <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:10" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="B9" s="109" t="s">
+      <c r="B9" s="122" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="78" t="s">
@@ -3144,68 +3192,68 @@
       <c r="D9" s="78" t="s">
         <v>167</v>
       </c>
-      <c r="E9" s="117" t="s">
+      <c r="E9" s="121" t="s">
         <v>168</v>
       </c>
-      <c r="F9" s="117"/>
+      <c r="F9" s="121"/>
       <c r="G9" s="74"/>
       <c r="H9" s="74"/>
-      <c r="I9" s="116"/>
-      <c r="J9" s="116"/>
+      <c r="I9" s="120"/>
+      <c r="J9" s="120"/>
     </row>
     <row r="10" spans="1:10" s="5" customFormat="1" ht="30" customHeight="1">
-      <c r="B10" s="109"/>
+      <c r="B10" s="122"/>
       <c r="C10" s="35" t="s">
         <v>165</v>
       </c>
       <c r="D10" s="79" t="s">
         <v>171</v>
       </c>
-      <c r="E10" s="115">
+      <c r="E10" s="119">
         <v>700</v>
       </c>
-      <c r="F10" s="115"/>
+      <c r="F10" s="119"/>
     </row>
     <row r="11" spans="1:10" s="5" customFormat="1" ht="30">
-      <c r="B11" s="109"/>
+      <c r="B11" s="122"/>
       <c r="C11" s="33" t="s">
         <v>169</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E11" s="103">
+      <c r="E11" s="106">
         <v>240</v>
       </c>
-      <c r="F11" s="103"/>
+      <c r="F11" s="106"/>
     </row>
     <row r="12" spans="1:10" s="5" customFormat="1" ht="30">
-      <c r="B12" s="109"/>
-      <c r="C12" s="115" t="s">
+      <c r="B12" s="122"/>
+      <c r="C12" s="119" t="s">
         <v>170</v>
       </c>
       <c r="D12" s="79" t="s">
         <v>173</v>
       </c>
-      <c r="E12" s="115">
+      <c r="E12" s="119">
         <v>10</v>
       </c>
-      <c r="F12" s="115"/>
+      <c r="F12" s="119"/>
     </row>
     <row r="13" spans="1:10" s="5" customFormat="1" ht="30">
-      <c r="B13" s="109"/>
-      <c r="C13" s="115"/>
+      <c r="B13" s="122"/>
+      <c r="C13" s="119"/>
       <c r="D13" s="79" t="s">
         <v>174</v>
       </c>
-      <c r="E13" s="115">
+      <c r="E13" s="119">
         <v>80</v>
       </c>
-      <c r="F13" s="115"/>
+      <c r="F13" s="119"/>
     </row>
     <row r="14" spans="1:10" s="5" customFormat="1" ht="60" customHeight="1">
-      <c r="B14" s="109"/>
-      <c r="C14" s="111" t="s">
+      <c r="B14" s="122"/>
+      <c r="C14" s="124" t="s">
         <v>181</v>
       </c>
       <c r="D14" s="67" t="s">
@@ -3219,8 +3267,8 @@
       </c>
     </row>
     <row r="15" spans="1:10" s="5" customFormat="1">
-      <c r="B15" s="109"/>
-      <c r="C15" s="111"/>
+      <c r="B15" s="122"/>
+      <c r="C15" s="124"/>
       <c r="D15" s="77" t="s">
         <v>197</v>
       </c>
@@ -3232,8 +3280,8 @@
       </c>
     </row>
     <row r="16" spans="1:10" s="5" customFormat="1">
-      <c r="B16" s="109"/>
-      <c r="C16" s="111"/>
+      <c r="B16" s="122"/>
+      <c r="C16" s="124"/>
       <c r="D16" s="75" t="s">
         <v>198</v>
       </c>
@@ -3245,8 +3293,8 @@
       </c>
     </row>
     <row r="17" spans="2:9" s="5" customFormat="1" ht="30">
-      <c r="B17" s="109"/>
-      <c r="C17" s="111"/>
+      <c r="B17" s="122"/>
+      <c r="C17" s="124"/>
       <c r="D17" s="70" t="s">
         <v>175</v>
       </c>
@@ -3258,82 +3306,82 @@
       </c>
     </row>
     <row r="18" spans="2:9" s="5" customFormat="1" ht="61" customHeight="1">
-      <c r="B18" s="109"/>
+      <c r="B18" s="122"/>
       <c r="C18" s="80" t="s">
         <v>184</v>
       </c>
       <c r="D18" s="79" t="s">
         <v>176</v>
       </c>
-      <c r="E18" s="115">
+      <c r="E18" s="119">
         <v>850</v>
       </c>
-      <c r="F18" s="115"/>
+      <c r="F18" s="119"/>
     </row>
     <row r="19" spans="2:9" s="5" customFormat="1" ht="30">
-      <c r="B19" s="109"/>
-      <c r="C19" s="103" t="s">
+      <c r="B19" s="122"/>
+      <c r="C19" s="106" t="s">
         <v>185</v>
       </c>
       <c r="D19" s="73" t="s">
         <v>177</v>
       </c>
-      <c r="E19" s="106">
+      <c r="E19" s="109">
         <v>200</v>
       </c>
-      <c r="F19" s="106"/>
+      <c r="F19" s="109"/>
     </row>
     <row r="20" spans="2:9" s="5" customFormat="1" ht="30">
-      <c r="B20" s="109"/>
-      <c r="C20" s="103"/>
+      <c r="B20" s="122"/>
+      <c r="C20" s="106"/>
       <c r="D20" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="E20" s="103">
+      <c r="E20" s="106">
         <v>370</v>
       </c>
-      <c r="F20" s="103"/>
+      <c r="F20" s="106"/>
     </row>
     <row r="21" spans="2:9" s="33" customFormat="1" ht="30">
-      <c r="B21" s="109"/>
-      <c r="C21" s="113" t="s">
+      <c r="B21" s="122"/>
+      <c r="C21" s="126" t="s">
         <v>187</v>
       </c>
       <c r="D21" s="79" t="s">
         <v>186</v>
       </c>
-      <c r="E21" s="115">
+      <c r="E21" s="119">
         <v>800</v>
       </c>
-      <c r="F21" s="115"/>
+      <c r="F21" s="119"/>
     </row>
     <row r="22" spans="2:9" s="5" customFormat="1" ht="30">
-      <c r="B22" s="109"/>
-      <c r="C22" s="113"/>
+      <c r="B22" s="122"/>
+      <c r="C22" s="126"/>
       <c r="D22" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="E22" s="115">
+      <c r="E22" s="119">
         <v>500</v>
       </c>
-      <c r="F22" s="115"/>
+      <c r="F22" s="119"/>
     </row>
     <row r="23" spans="2:9" ht="30">
-      <c r="B23" s="109"/>
+      <c r="B23" s="122"/>
       <c r="C23" s="1" t="s">
         <v>188</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E23" s="114">
+      <c r="E23" s="118">
         <v>350</v>
       </c>
-      <c r="F23" s="114"/>
+      <c r="F23" s="118"/>
     </row>
     <row r="24" spans="2:9" s="5" customFormat="1"/>
     <row r="25" spans="2:9" ht="54" customHeight="1">
-      <c r="B25" s="95" t="s">
+      <c r="B25" s="115" t="s">
         <v>142</v>
       </c>
       <c r="C25" s="83" t="s">
@@ -3359,7 +3407,7 @@
       </c>
     </row>
     <row r="26" spans="2:9" ht="30" customHeight="1">
-      <c r="B26" s="95"/>
+      <c r="B26" s="115"/>
       <c r="C26" s="81" t="s">
         <v>165</v>
       </c>
@@ -3383,7 +3431,7 @@
       </c>
     </row>
     <row r="27" spans="2:9" ht="32" customHeight="1">
-      <c r="B27" s="95"/>
+      <c r="B27" s="115"/>
       <c r="C27" s="5" t="s">
         <v>169</v>
       </c>
@@ -3407,8 +3455,8 @@
       </c>
     </row>
     <row r="28" spans="2:9" ht="32" customHeight="1">
-      <c r="B28" s="95"/>
-      <c r="C28" s="110" t="s">
+      <c r="B28" s="115"/>
+      <c r="C28" s="123" t="s">
         <v>170</v>
       </c>
       <c r="D28" s="86" t="s">
@@ -3431,8 +3479,8 @@
       </c>
     </row>
     <row r="29" spans="2:9" ht="32" customHeight="1">
-      <c r="B29" s="95"/>
-      <c r="C29" s="110"/>
+      <c r="B29" s="115"/>
+      <c r="C29" s="123"/>
       <c r="D29" s="84" t="s">
         <v>174</v>
       </c>
@@ -3453,7 +3501,7 @@
       </c>
     </row>
     <row r="30" spans="2:9" ht="47" customHeight="1">
-      <c r="B30" s="95"/>
+      <c r="B30" s="115"/>
       <c r="C30" s="67" t="s">
         <v>195</v>
       </c>
@@ -3477,7 +3525,7 @@
       </c>
     </row>
     <row r="31" spans="2:9" ht="32" customHeight="1">
-      <c r="B31" s="95"/>
+      <c r="B31" s="115"/>
       <c r="C31" s="81" t="s">
         <v>185</v>
       </c>
@@ -3501,11 +3549,11 @@
       </c>
     </row>
     <row r="32" spans="2:9" ht="30" customHeight="1">
-      <c r="B32" s="95"/>
+      <c r="B32" s="115"/>
       <c r="C32" s="85" t="s">
         <v>201</v>
       </c>
-      <c r="D32" s="111" t="s">
+      <c r="D32" s="124" t="s">
         <v>178</v>
       </c>
       <c r="E32" s="68">
@@ -3525,11 +3573,11 @@
       </c>
     </row>
     <row r="33" spans="2:9" ht="23" customHeight="1">
-      <c r="B33" s="95"/>
+      <c r="B33" s="115"/>
       <c r="C33" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="D33" s="111"/>
+      <c r="D33" s="124"/>
       <c r="E33" s="33">
         <v>20</v>
       </c>
@@ -3547,8 +3595,8 @@
       </c>
     </row>
     <row r="34" spans="2:9" ht="32" customHeight="1">
-      <c r="B34" s="95"/>
-      <c r="C34" s="112" t="s">
+      <c r="B34" s="115"/>
+      <c r="C34" s="125" t="s">
         <v>203</v>
       </c>
       <c r="D34" s="86" t="s">
@@ -3571,8 +3619,8 @@
       </c>
     </row>
     <row r="35" spans="2:9" ht="32" customHeight="1">
-      <c r="B35" s="95"/>
-      <c r="C35" s="112"/>
+      <c r="B35" s="115"/>
+      <c r="C35" s="125"/>
       <c r="D35" s="84" t="s">
         <v>204</v>
       </c>
@@ -3593,7 +3641,7 @@
       </c>
     </row>
     <row r="36" spans="2:9" ht="32" customHeight="1">
-      <c r="B36" s="95"/>
+      <c r="B36" s="115"/>
       <c r="C36" s="67" t="s">
         <v>205</v>
       </c>
@@ -3618,6 +3666,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B9:B23"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="B25:B36"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="C19:C20"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E21:F21"/>
@@ -3630,15 +3687,6 @@
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E9:F9"/>
-    <mergeCell ref="B9:B23"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="B25:B36"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="C19:C20"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -3679,48 +3727,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:21">
-      <c r="B1" s="124" t="s">
+      <c r="B1" s="127" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="124"/>
+      <c r="C1" s="127"/>
     </row>
     <row r="4" spans="2:21" s="4" customFormat="1">
-      <c r="B4" s="121" t="s">
+      <c r="B4" s="133" t="s">
         <v>118</v>
       </c>
-      <c r="C4" s="121"/>
-      <c r="D4" s="123" t="s">
+      <c r="C4" s="133"/>
+      <c r="D4" s="135" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="123"/>
-      <c r="F4" s="123"/>
-      <c r="G4" s="123"/>
-      <c r="H4" s="126" t="s">
+      <c r="E4" s="135"/>
+      <c r="F4" s="135"/>
+      <c r="G4" s="135"/>
+      <c r="H4" s="129" t="s">
         <v>119</v>
       </c>
-      <c r="I4" s="126"/>
-      <c r="J4" s="126"/>
-      <c r="K4" s="126"/>
-      <c r="L4" s="126"/>
-      <c r="M4" s="122" t="s">
+      <c r="I4" s="129"/>
+      <c r="J4" s="129"/>
+      <c r="K4" s="129"/>
+      <c r="L4" s="129"/>
+      <c r="M4" s="134" t="s">
         <v>120</v>
       </c>
-      <c r="N4" s="122"/>
-      <c r="O4" s="122"/>
-      <c r="P4" s="122"/>
-      <c r="Q4" s="122"/>
-      <c r="R4" s="122"/>
-      <c r="S4" s="118" t="s">
+      <c r="N4" s="134"/>
+      <c r="O4" s="134"/>
+      <c r="P4" s="134"/>
+      <c r="Q4" s="134"/>
+      <c r="R4" s="134"/>
+      <c r="S4" s="130" t="s">
         <v>121</v>
       </c>
-      <c r="T4" s="118"/>
-      <c r="U4" s="118"/>
+      <c r="T4" s="130"/>
+      <c r="U4" s="130"/>
     </row>
     <row r="5" spans="2:21" s="7" customFormat="1" ht="60">
-      <c r="B5" s="125" t="s">
+      <c r="B5" s="128" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="125"/>
+      <c r="C5" s="128"/>
       <c r="D5" s="8" t="s">
         <v>39</v>
       </c>
@@ -3777,10 +3825,10 @@
       </c>
     </row>
     <row r="6" spans="2:21" s="11" customFormat="1">
-      <c r="B6" s="125" t="s">
+      <c r="B6" s="128" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="125"/>
+      <c r="C6" s="128"/>
       <c r="D6" s="12" t="s">
         <v>45</v>
       </c>
@@ -3837,10 +3885,10 @@
       </c>
     </row>
     <row r="7" spans="2:21" s="11" customFormat="1" ht="75">
-      <c r="B7" s="125" t="s">
+      <c r="B7" s="128" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="125"/>
+      <c r="C7" s="128"/>
       <c r="D7" s="13" t="s">
         <v>50</v>
       </c>
@@ -3897,10 +3945,10 @@
       </c>
     </row>
     <row r="8" spans="2:21" s="15" customFormat="1" ht="60">
-      <c r="B8" s="125" t="s">
+      <c r="B8" s="128" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="125"/>
+      <c r="C8" s="128"/>
       <c r="D8" s="14" t="s">
         <v>48</v>
       </c>
@@ -3951,10 +3999,10 @@
       </c>
     </row>
     <row r="9" spans="2:21" s="15" customFormat="1" ht="142" customHeight="1">
-      <c r="B9" s="125" t="s">
+      <c r="B9" s="128" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="125"/>
+      <c r="C9" s="128"/>
       <c r="D9" s="14" t="s">
         <v>61</v>
       </c>
@@ -4011,10 +4059,10 @@
       </c>
     </row>
     <row r="10" spans="2:21" s="18" customFormat="1">
-      <c r="B10" s="121" t="s">
+      <c r="B10" s="133" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="121"/>
+      <c r="C10" s="133"/>
       <c r="D10" s="16">
         <v>512</v>
       </c>
@@ -4063,10 +4111,10 @@
       </c>
     </row>
     <row r="11" spans="2:21" s="18" customFormat="1">
-      <c r="B11" s="119" t="s">
+      <c r="B11" s="131" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="120"/>
+      <c r="C11" s="132"/>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
       <c r="F11" s="23"/>
@@ -4111,10 +4159,10 @@
       </c>
     </row>
     <row r="12" spans="2:21" s="18" customFormat="1">
-      <c r="B12" s="119" t="s">
+      <c r="B12" s="131" t="s">
         <v>82</v>
       </c>
-      <c r="C12" s="120"/>
+      <c r="C12" s="132"/>
       <c r="D12" s="24" t="s">
         <v>84</v>
       </c>
@@ -4169,10 +4217,10 @@
       </c>
     </row>
     <row r="13" spans="2:21" s="18" customFormat="1">
-      <c r="B13" s="121" t="s">
+      <c r="B13" s="133" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="121"/>
+      <c r="C13" s="133"/>
       <c r="D13" s="16" t="s">
         <v>58</v>
       </c>
@@ -4223,7 +4271,7 @@
       </c>
     </row>
     <row r="14" spans="2:21" s="18" customFormat="1" ht="30">
-      <c r="B14" s="121" t="s">
+      <c r="B14" s="133" t="s">
         <v>35</v>
       </c>
       <c r="C14" s="31" t="s">
@@ -4263,7 +4311,7 @@
       <c r="U14" s="17"/>
     </row>
     <row r="15" spans="2:21" s="10" customFormat="1" ht="105">
-      <c r="B15" s="121"/>
+      <c r="B15" s="133"/>
       <c r="C15" s="32" t="s">
         <v>132</v>
       </c>
@@ -4305,10 +4353,10 @@
       </c>
     </row>
     <row r="16" spans="2:21" s="10" customFormat="1" ht="45">
-      <c r="B16" s="121" t="s">
+      <c r="B16" s="133" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="121"/>
+      <c r="C16" s="133"/>
       <c r="D16" s="19" t="s">
         <v>55</v>
       </c>
@@ -4360,13 +4408,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="H4:L4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
     <mergeCell ref="S4:U4"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B14:B15"/>
@@ -4377,6 +4418,13 @@
     <mergeCell ref="M4:R4"/>
     <mergeCell ref="D4:G4"/>
     <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="H4:L4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -4391,8 +4439,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4410,136 +4461,150 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:8">
-      <c r="B3" s="127" t="s">
+      <c r="B3" s="92" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="128" t="s">
+      <c r="C3" s="93" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="129" t="s">
+      <c r="D3" s="136" t="s">
         <v>208</v>
       </c>
-      <c r="E3" s="129"/>
-      <c r="F3" s="129"/>
-      <c r="G3" s="129"/>
-      <c r="H3" s="129"/>
-    </row>
-    <row r="4" spans="1:8" s="91" customFormat="1" ht="60">
-      <c r="B4" s="130" t="s">
+      <c r="E3" s="136"/>
+      <c r="F3" s="136"/>
+      <c r="G3" s="136"/>
+      <c r="H3" s="136"/>
+    </row>
+    <row r="4" spans="1:8" s="91" customFormat="1" ht="45">
+      <c r="B4" s="94" t="s">
         <v>37</v>
       </c>
       <c r="C4" s="25" t="s">
         <v>211</v>
       </c>
-      <c r="D4" s="131" t="s">
+      <c r="D4" s="95" t="s">
         <v>210</v>
       </c>
-      <c r="E4" s="131" t="s">
+      <c r="E4" s="95" t="s">
         <v>212</v>
       </c>
-      <c r="F4" s="131" t="s">
+      <c r="F4" s="95" t="s">
         <v>213</v>
       </c>
-      <c r="G4" s="131" t="s">
+      <c r="G4" s="95" t="s">
         <v>214</v>
       </c>
-      <c r="H4" s="131" t="s">
-        <v>222</v>
+      <c r="H4" s="95" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="75">
-      <c r="B5" s="127" t="s">
+      <c r="B5" s="92" t="s">
         <v>207</v>
       </c>
-      <c r="C5" s="132" t="s">
+      <c r="C5" s="96" t="s">
         <v>215</v>
       </c>
-      <c r="D5" s="133" t="s">
+      <c r="D5" s="97" t="s">
         <v>219</v>
       </c>
-      <c r="E5" s="133" t="s">
+      <c r="E5" s="97" t="s">
         <v>218</v>
       </c>
-      <c r="F5" s="133" t="s">
+      <c r="F5" s="97" t="s">
         <v>220</v>
       </c>
-      <c r="G5" s="134" t="s">
+      <c r="G5" s="98" t="s">
         <v>221</v>
       </c>
-      <c r="H5" s="135"/>
+      <c r="H5" s="98" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="30">
-      <c r="B6" s="130" t="s">
+      <c r="B6" s="94" t="s">
         <v>217</v>
       </c>
-      <c r="C6" s="135" t="s">
+      <c r="C6" s="137" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="135" t="s">
+      <c r="D6" s="139" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="135" t="s">
+      <c r="E6" s="139" t="s">
         <v>68</v>
       </c>
-      <c r="F6" s="135" t="s">
+      <c r="F6" s="139" t="s">
         <v>68</v>
       </c>
-      <c r="G6" s="135" t="s">
+      <c r="G6" s="139" t="s">
         <v>68</v>
       </c>
-      <c r="H6" s="135" t="s">
+      <c r="H6" s="139" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="60">
-      <c r="B7" s="127" t="s">
+    <row r="7" spans="1:8" ht="75">
+      <c r="B7" s="92" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="136" t="s">
+      <c r="C7" s="100" t="s">
         <v>216</v>
       </c>
-      <c r="D7" s="136" t="s">
+      <c r="D7" s="100" t="s">
+        <v>226</v>
+      </c>
+      <c r="E7" s="99"/>
+      <c r="F7" s="99"/>
+      <c r="G7" s="99" t="s">
+        <v>231</v>
+      </c>
+      <c r="H7" s="100" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="240">
+      <c r="B8" s="92" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="138" t="s">
+        <v>223</v>
+      </c>
+      <c r="D8" s="140" t="s">
+        <v>225</v>
+      </c>
+      <c r="E8" s="140" t="s">
         <v>227</v>
       </c>
-      <c r="E7" s="135"/>
-      <c r="F7" s="135"/>
-      <c r="G7" s="135"/>
-      <c r="H7" s="135"/>
-    </row>
-    <row r="8" spans="1:8" ht="150">
-      <c r="B8" s="127" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="136" t="s">
-        <v>224</v>
-      </c>
-      <c r="D8" s="136" t="s">
-        <v>226</v>
-      </c>
-      <c r="E8" s="136" t="s">
+      <c r="F8" s="140" t="s">
         <v>228</v>
       </c>
-      <c r="F8" s="135"/>
-      <c r="G8" s="135"/>
-      <c r="H8" s="135"/>
+      <c r="G8" s="140" t="s">
+        <v>232</v>
+      </c>
+      <c r="H8" s="141" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="90" t="s">
         <v>209</v>
       </c>
-      <c r="B9" s="127" t="s">
+      <c r="B9" s="92" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="135" t="s">
-        <v>223</v>
-      </c>
-      <c r="D9" s="135" t="s">
-        <v>225</v>
-      </c>
-      <c r="E9" s="135"/>
-      <c r="F9" s="135"/>
-      <c r="G9" s="135"/>
-      <c r="H9" s="135"/>
+      <c r="C9" s="99" t="s">
+        <v>222</v>
+      </c>
+      <c r="D9" s="99" t="s">
+        <v>224</v>
+      </c>
+      <c r="E9" s="99" t="s">
+        <v>230</v>
+      </c>
+      <c r="F9" s="99"/>
+      <c r="G9" s="99"/>
+      <c r="H9" s="99"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>